<commit_message>
Dodanie planu testów w zakresie menu głównego
</commit_message>
<xml_diff>
--- a/Test.xlsx
+++ b/Test.xlsx
@@ -8,15 +8,16 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Marek\Documents\GitHub\Testy [Dołącz-Mises]\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FAA75C82-7746-4E6F-BF19-98953C2F7880}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6C4786CB-8F10-4F6F-AA1F-233F0C1CCFBB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17640" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17640" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Projekt" sheetId="1" r:id="rId1"/>
     <sheet name="Kompilacja" sheetId="2" state="hidden" r:id="rId2"/>
     <sheet name="Wymagania" sheetId="4" state="hidden" r:id="rId3"/>
     <sheet name="Dołącz - rejestracja" sheetId="6" r:id="rId4"/>
+    <sheet name="Menu główne" sheetId="7" r:id="rId5"/>
   </sheets>
   <calcPr calcId="152511"/>
   <extLst>
@@ -28,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="328" uniqueCount="156">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="518" uniqueCount="209">
   <si>
     <t>Nazwa</t>
   </si>
@@ -521,6 +522,166 @@
     <t>Uwaga dotyczy tylko 1 błędu:
 Niestety nie umiem wskazać jednoznacznejścieżki do błędu.
 Wydaje się, że jest związany z niepoprawnym adresem email, ale nie jest to regułą.</t>
+  </si>
+  <si>
+    <t>2_1</t>
+  </si>
+  <si>
+    <t>Dostęp do interneteu, uruchomiona strona główna</t>
+  </si>
+  <si>
+    <t>Zostaje otwarta strona https://mises.pl/artykuly</t>
+  </si>
+  <si>
+    <t>Zostaje otwarta strona https://mises.pl/ebooki</t>
+  </si>
+  <si>
+    <t>Zostaje otwarta strona https://mises.pl/#projects</t>
+  </si>
+  <si>
+    <t>Zostaje otwarta strona https://www.mises.sklep.pl/</t>
+  </si>
+  <si>
+    <t>Zostaje otwarta strona https://mises.pl/o-nas</t>
+  </si>
+  <si>
+    <t>Otwarcie strony "o nas"</t>
+  </si>
+  <si>
+    <t>Zostaje otwarta strona https://mises.pl/kontakt</t>
+  </si>
+  <si>
+    <t>Powrót do strony głównej</t>
+  </si>
+  <si>
+    <t>Zostaje otwarta strona https://mises.pl/wsparcie</t>
+  </si>
+  <si>
+    <t>Zostaje otwarta strona https://dolacz.mises.pl/</t>
+  </si>
+  <si>
+    <t>Pasek nawigacyjny</t>
+  </si>
+  <si>
+    <t>Zostaje otwarta strona https://raporty.mises.pl/</t>
+  </si>
+  <si>
+    <t>Otwarcie strony "sklep"</t>
+  </si>
+  <si>
+    <t>Otwarcie strony "Kontakt"</t>
+  </si>
+  <si>
+    <t>Otwarcie strony "Wesprzyj nas"</t>
+  </si>
+  <si>
+    <t>Otwarcie strony "Dołącz"</t>
+  </si>
+  <si>
+    <t>Zostaje otwarta strona https://mises.pl</t>
+  </si>
+  <si>
+    <t>Otwarcie strony "Raporty"</t>
+  </si>
+  <si>
+    <t>Otwarcie strony "Projekty"</t>
+  </si>
+  <si>
+    <t>Otwarcie strony "Eboki"</t>
+  </si>
+  <si>
+    <t>Otwarcie strony "Artykuły"</t>
+  </si>
+  <si>
+    <t>Zostaje otwarta pod strona https://mises.pl/#projects</t>
+  </si>
+  <si>
+    <t>Niespójny z wcześniejszymi podstronami link</t>
+  </si>
+  <si>
+    <t>USTERKA PODRZĘDNA</t>
+  </si>
+  <si>
+    <t>Brak menu głównego</t>
+  </si>
+  <si>
+    <t>Brak możliwości powrotu do strony głównej z poziomu menu strony, powrót do strony głównej tylko przez menu przeglądarki</t>
+  </si>
+  <si>
+    <t>USTERKA</t>
+  </si>
+  <si>
+    <t>Brak możliwości powrotu do strony głównej z poziomu menu strony, powrót do strony głównej tylko przez zamknięcie podstrony</t>
+  </si>
+  <si>
+    <t>Niespójny layout strony</t>
+  </si>
+  <si>
+    <t>Niespójna logika strony. Zostaje otwarta nowa karta, inny layout menu w karcie, niedziałający link logo. Niespójne logo.</t>
+  </si>
+  <si>
+    <t>Niespójna logika strony. Link do strony głównej otwiera nową kartę zamiast powrócić do już otwartej.</t>
+  </si>
+  <si>
+    <t>Kontrola działania nawigacji ze strony paska nawigacyjnego strony głównej</t>
+  </si>
+  <si>
+    <t>2023-08-24 
+11:50:00</t>
+  </si>
+  <si>
+    <t>Menu spójne ze stroną główną</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Powrót do strony głównej przez kliknięcie w logo firmy </t>
+  </si>
+  <si>
+    <t>Weryfikacja layoutu</t>
+  </si>
+  <si>
+    <t>Powrót do strony głównej przez funkcję powrotu przeglądarki</t>
+  </si>
+  <si>
+    <t>Zostaje otwarta strona https://www.mises.sklep.pl/ w aktualnej karcie</t>
+  </si>
+  <si>
+    <t>Zmknięcie karty "Sklep"</t>
+  </si>
+  <si>
+    <t>Pozostaje otwarta karta ze stroną główną</t>
+  </si>
+  <si>
+    <t>Otwarcie strony "Sklep"</t>
+  </si>
+  <si>
+    <t>Menu niespójne ze stroną główną</t>
+  </si>
+  <si>
+    <t>Odświerzenie strony https://raporty.mises.pl/</t>
+  </si>
+  <si>
+    <t>Zostaje otwarta strona https://www.mises.sklep.pl/ w nowej karcie</t>
+  </si>
+  <si>
+    <t>Odświerzenie strony https://www.mises.sklep.p</t>
+  </si>
+  <si>
+    <t>Zostaje otwarta strona https://dolacz.mises.pl/ na karcie głównej</t>
+  </si>
+  <si>
+    <t>Zostaje otwarta strona https://dolacz.mises.pl/ w nowej karcie</t>
+  </si>
+  <si>
+    <t>Niedostępna funkcja przeglądarki</t>
+  </si>
+  <si>
+    <t>Niespójne layout menu. Niespójne logo firmy</t>
+  </si>
+  <si>
+    <t>Niespójna logika strony.</t>
+  </si>
+  <si>
+    <t>Niewłaściwa logika strony</t>
   </si>
 </sst>
 </file>
@@ -752,7 +913,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="59">
+  <cellXfs count="60">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -795,51 +956,6 @@
     <xf numFmtId="14" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="22" fontId="2" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="22" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="22" fontId="2" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="5" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -851,18 +967,87 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="22" fontId="2" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="22" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="22" fontId="2" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="5" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="10" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -875,26 +1060,8 @@
     <xf numFmtId="0" fontId="7" fillId="0" borderId="10" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="16" fontId="2" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -903,13 +1070,10 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -917,18 +1081,7 @@
     <cellStyle name="Hiperłącze" xfId="1" builtinId="8"/>
     <cellStyle name="Normalny" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="47">
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="7" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
+  <dxfs count="22">
     <dxf>
       <font>
         <b/>
@@ -1042,17 +1195,6 @@
       <font>
         <b/>
         <i val="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF7C80"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
         <color rgb="FFFF0000"/>
       </font>
       <fill>
@@ -1133,214 +1275,6 @@
       <fill>
         <patternFill>
           <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <color theme="5" tint="-0.499984740745262"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF9966"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF6464"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF7C80"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF3300"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF92D050"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF92D050"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF7C80"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF3300"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF92D050"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF92D050"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF3300"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF92D050"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF92D050"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
         </patternFill>
       </fill>
     </dxf>
@@ -1661,10 +1595,10 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A1" s="16" t="s">
+      <c r="A1" s="33" t="s">
         <v>32</v>
       </c>
-      <c r="B1" s="16"/>
+      <c r="B1" s="33"/>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" s="9" t="s">
@@ -1719,10 +1653,10 @@
       <c r="B8" s="9"/>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A10" s="16" t="s">
+      <c r="A10" s="33" t="s">
         <v>33</v>
       </c>
-      <c r="B10" s="16"/>
+      <c r="B10" s="33"/>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A11" s="9" t="s">
@@ -1757,7 +1691,7 @@
       </c>
     </row>
     <row r="15" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="17" t="s">
+      <c r="A15" s="34" t="s">
         <v>41</v>
       </c>
       <c r="B15" s="15" t="s">
@@ -1765,47 +1699,47 @@
       </c>
     </row>
     <row r="16" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="17"/>
+      <c r="A16" s="34"/>
       <c r="B16" s="12"/>
     </row>
     <row r="17" spans="1:1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="17"/>
+      <c r="A17" s="34"/>
     </row>
     <row r="18" spans="1:1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A18" s="17"/>
+      <c r="A18" s="34"/>
     </row>
     <row r="19" spans="1:1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A19" s="17"/>
+      <c r="A19" s="34"/>
     </row>
     <row r="20" spans="1:1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A20" s="17"/>
+      <c r="A20" s="34"/>
     </row>
     <row r="21" spans="1:1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A21" s="17"/>
+      <c r="A21" s="34"/>
     </row>
     <row r="22" spans="1:1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A22" s="17"/>
+      <c r="A22" s="34"/>
     </row>
     <row r="23" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A23" s="17"/>
+      <c r="A23" s="34"/>
     </row>
     <row r="24" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A24" s="17"/>
+      <c r="A24" s="34"/>
     </row>
     <row r="25" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A25" s="17"/>
+      <c r="A25" s="34"/>
     </row>
     <row r="26" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A26" s="17"/>
+      <c r="A26" s="34"/>
     </row>
     <row r="27" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A27" s="17"/>
+      <c r="A27" s="34"/>
     </row>
     <row r="28" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A28" s="17"/>
+      <c r="A28" s="34"/>
     </row>
     <row r="29" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A29" s="17"/>
+      <c r="A29" s="34"/>
     </row>
   </sheetData>
   <mergeCells count="3">
@@ -1949,10 +1883,10 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="J1 I1:I1048576">
-    <cfRule type="cellIs" dxfId="46" priority="1" operator="equal">
+    <cfRule type="cellIs" dxfId="21" priority="1" operator="equal">
       <formula>"TAK"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="45" priority="2" operator="equal">
+    <cfRule type="cellIs" dxfId="20" priority="2" operator="equal">
       <formula>"NIE"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -1970,11 +1904,11 @@
   <sheetPr codeName="Arkusz4"/>
   <dimension ref="A1:S53"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="2" ySplit="1" topLeftCell="C30" activePane="bottomRight" state="frozen"/>
+    <sheetView workbookViewId="0">
+      <pane xSplit="2" ySplit="1" topLeftCell="C2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="D26" sqref="D26:D34"/>
+      <selection pane="bottomRight" activeCell="D44" sqref="D44:D53"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.2"/>
@@ -1988,20 +1922,20 @@
     <col min="7" max="7" width="10.28515625" style="4" customWidth="1"/>
     <col min="8" max="8" width="9" style="4" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="6.42578125" style="4" customWidth="1"/>
-    <col min="10" max="10" width="1.7109375" style="39" customWidth="1"/>
+    <col min="10" max="10" width="1.7109375" style="22" customWidth="1"/>
     <col min="11" max="11" width="5" style="4" customWidth="1"/>
     <col min="12" max="12" width="22.85546875" style="4" customWidth="1"/>
     <col min="13" max="13" width="26.85546875" style="4" customWidth="1"/>
     <col min="14" max="14" width="25.140625" style="4" customWidth="1"/>
     <col min="15" max="15" width="5.85546875" style="4" customWidth="1"/>
     <col min="16" max="16" width="14.42578125" style="4" customWidth="1"/>
-    <col min="17" max="17" width="14.42578125" style="48" customWidth="1"/>
+    <col min="17" max="17" width="14.42578125" style="26" customWidth="1"/>
     <col min="18" max="18" width="14.42578125" style="4" customWidth="1"/>
     <col min="19" max="19" width="22.85546875" style="4" customWidth="1"/>
-    <col min="20" max="16384" width="9.140625" style="35"/>
+    <col min="20" max="16384" width="9.140625" style="20"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:19" s="31" customFormat="1" ht="24.75" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:19" s="16" customFormat="1" ht="24.75" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A1" s="7" t="s">
         <v>14</v>
       </c>
@@ -2029,7 +1963,7 @@
       <c r="I1" s="6" t="s">
         <v>24</v>
       </c>
-      <c r="J1" s="32"/>
+      <c r="J1" s="17"/>
       <c r="K1" s="6" t="s">
         <v>29</v>
       </c>
@@ -2048,43 +1982,43 @@
       <c r="P1" s="6" t="s">
         <v>22</v>
       </c>
-      <c r="Q1" s="46" t="s">
+      <c r="Q1" s="24" t="s">
         <v>25</v>
       </c>
-      <c r="R1" s="33" t="s">
+      <c r="R1" s="18" t="s">
         <v>23</v>
       </c>
-      <c r="S1" s="34"/>
+      <c r="S1" s="19"/>
     </row>
     <row r="2" spans="1:19" ht="24" x14ac:dyDescent="0.2">
-      <c r="A2" s="27">
+      <c r="A2" s="38">
         <v>1</v>
       </c>
-      <c r="B2" s="21" t="s">
-        <v>46</v>
-      </c>
-      <c r="C2" s="21" t="s">
+      <c r="B2" s="41" t="s">
+        <v>46</v>
+      </c>
+      <c r="C2" s="41" t="s">
         <v>49</v>
       </c>
-      <c r="D2" s="21" t="s">
+      <c r="D2" s="41" t="s">
         <v>57</v>
       </c>
-      <c r="E2" s="21" t="s">
+      <c r="E2" s="41" t="s">
         <v>50</v>
       </c>
-      <c r="F2" s="21">
+      <c r="F2" s="41">
         <v>1</v>
       </c>
-      <c r="G2" s="21" t="s">
+      <c r="G2" s="41" t="s">
         <v>45</v>
       </c>
-      <c r="H2" s="24" t="s">
+      <c r="H2" s="44" t="s">
         <v>142</v>
       </c>
-      <c r="I2" s="36" t="s">
+      <c r="I2" s="47" t="s">
         <v>81</v>
       </c>
-      <c r="J2" s="37"/>
+      <c r="J2" s="21"/>
       <c r="K2" s="13">
         <v>1</v>
       </c>
@@ -2101,21 +2035,21 @@
         <v>46</v>
       </c>
       <c r="P2" s="13"/>
-      <c r="Q2" s="47"/>
-      <c r="R2" s="18" t="s">
+      <c r="Q2" s="25"/>
+      <c r="R2" s="35" t="s">
         <v>82</v>
       </c>
     </row>
     <row r="3" spans="1:19" ht="24" x14ac:dyDescent="0.2">
-      <c r="A3" s="28"/>
-      <c r="B3" s="22"/>
-      <c r="C3" s="22"/>
-      <c r="D3" s="22"/>
-      <c r="E3" s="22"/>
-      <c r="F3" s="22"/>
-      <c r="G3" s="22"/>
-      <c r="H3" s="25"/>
-      <c r="I3" s="38"/>
+      <c r="A3" s="39"/>
+      <c r="B3" s="42"/>
+      <c r="C3" s="42"/>
+      <c r="D3" s="42"/>
+      <c r="E3" s="42"/>
+      <c r="F3" s="42"/>
+      <c r="G3" s="42"/>
+      <c r="H3" s="45"/>
+      <c r="I3" s="48"/>
       <c r="K3" s="4">
         <v>2</v>
       </c>
@@ -2131,18 +2065,18 @@
       <c r="O3" s="4" t="s">
         <v>46</v>
       </c>
-      <c r="R3" s="19"/>
+      <c r="R3" s="36"/>
     </row>
     <row r="4" spans="1:19" ht="36" x14ac:dyDescent="0.2">
-      <c r="A4" s="28"/>
-      <c r="B4" s="22"/>
-      <c r="C4" s="22"/>
-      <c r="D4" s="22"/>
-      <c r="E4" s="22"/>
-      <c r="F4" s="22"/>
-      <c r="G4" s="22"/>
-      <c r="H4" s="25"/>
-      <c r="I4" s="38"/>
+      <c r="A4" s="39"/>
+      <c r="B4" s="42"/>
+      <c r="C4" s="42"/>
+      <c r="D4" s="42"/>
+      <c r="E4" s="42"/>
+      <c r="F4" s="42"/>
+      <c r="G4" s="42"/>
+      <c r="H4" s="45"/>
+      <c r="I4" s="48"/>
       <c r="K4" s="4">
         <v>3</v>
       </c>
@@ -2158,18 +2092,18 @@
       <c r="O4" s="4" t="s">
         <v>46</v>
       </c>
-      <c r="R4" s="19"/>
+      <c r="R4" s="36"/>
     </row>
     <row r="5" spans="1:19" ht="36" x14ac:dyDescent="0.2">
-      <c r="A5" s="28"/>
-      <c r="B5" s="22"/>
-      <c r="C5" s="22"/>
-      <c r="D5" s="22"/>
-      <c r="E5" s="22"/>
-      <c r="F5" s="22"/>
-      <c r="G5" s="22"/>
-      <c r="H5" s="25"/>
-      <c r="I5" s="38"/>
+      <c r="A5" s="39"/>
+      <c r="B5" s="42"/>
+      <c r="C5" s="42"/>
+      <c r="D5" s="42"/>
+      <c r="E5" s="42"/>
+      <c r="F5" s="42"/>
+      <c r="G5" s="42"/>
+      <c r="H5" s="45"/>
+      <c r="I5" s="48"/>
       <c r="K5" s="4">
         <v>4</v>
       </c>
@@ -2185,18 +2119,18 @@
       <c r="O5" s="4" t="s">
         <v>46</v>
       </c>
-      <c r="R5" s="19"/>
+      <c r="R5" s="36"/>
     </row>
     <row r="6" spans="1:19" ht="24" x14ac:dyDescent="0.2">
-      <c r="A6" s="28"/>
-      <c r="B6" s="22"/>
-      <c r="C6" s="22"/>
-      <c r="D6" s="22"/>
-      <c r="E6" s="22"/>
-      <c r="F6" s="22"/>
-      <c r="G6" s="22"/>
-      <c r="H6" s="25"/>
-      <c r="I6" s="38"/>
+      <c r="A6" s="39"/>
+      <c r="B6" s="42"/>
+      <c r="C6" s="42"/>
+      <c r="D6" s="42"/>
+      <c r="E6" s="42"/>
+      <c r="F6" s="42"/>
+      <c r="G6" s="42"/>
+      <c r="H6" s="45"/>
+      <c r="I6" s="48"/>
       <c r="K6" s="4">
         <v>5</v>
       </c>
@@ -2212,18 +2146,18 @@
       <c r="O6" s="4" t="s">
         <v>46</v>
       </c>
-      <c r="R6" s="19"/>
+      <c r="R6" s="36"/>
     </row>
     <row r="7" spans="1:19" ht="48" x14ac:dyDescent="0.2">
-      <c r="A7" s="28"/>
-      <c r="B7" s="22"/>
-      <c r="C7" s="22"/>
-      <c r="D7" s="22"/>
-      <c r="E7" s="22"/>
-      <c r="F7" s="22"/>
-      <c r="G7" s="22"/>
-      <c r="H7" s="25"/>
-      <c r="I7" s="38"/>
+      <c r="A7" s="39"/>
+      <c r="B7" s="42"/>
+      <c r="C7" s="42"/>
+      <c r="D7" s="42"/>
+      <c r="E7" s="42"/>
+      <c r="F7" s="42"/>
+      <c r="G7" s="42"/>
+      <c r="H7" s="45"/>
+      <c r="I7" s="48"/>
       <c r="K7" s="4">
         <v>6</v>
       </c>
@@ -2239,19 +2173,19 @@
       <c r="O7" s="4" t="s">
         <v>46</v>
       </c>
-      <c r="R7" s="19"/>
+      <c r="R7" s="36"/>
     </row>
     <row r="8" spans="1:19" ht="24.75" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="29"/>
-      <c r="B8" s="23"/>
-      <c r="C8" s="23"/>
-      <c r="D8" s="23"/>
-      <c r="E8" s="23"/>
-      <c r="F8" s="23"/>
-      <c r="G8" s="23"/>
-      <c r="H8" s="26"/>
-      <c r="I8" s="40"/>
-      <c r="J8" s="41"/>
+      <c r="A8" s="40"/>
+      <c r="B8" s="43"/>
+      <c r="C8" s="43"/>
+      <c r="D8" s="43"/>
+      <c r="E8" s="43"/>
+      <c r="F8" s="43"/>
+      <c r="G8" s="43"/>
+      <c r="H8" s="46"/>
+      <c r="I8" s="49"/>
+      <c r="J8" s="23"/>
       <c r="K8" s="14">
         <v>7</v>
       </c>
@@ -2268,38 +2202,38 @@
         <v>46</v>
       </c>
       <c r="P8" s="14"/>
-      <c r="Q8" s="49"/>
-      <c r="R8" s="20"/>
+      <c r="Q8" s="27"/>
+      <c r="R8" s="37"/>
     </row>
     <row r="9" spans="1:19" x14ac:dyDescent="0.2">
-      <c r="A9" s="27">
+      <c r="A9" s="38">
         <v>2</v>
       </c>
-      <c r="B9" s="21" t="s">
+      <c r="B9" s="41" t="s">
         <v>89</v>
       </c>
-      <c r="C9" s="21" t="s">
+      <c r="C9" s="41" t="s">
         <v>49</v>
       </c>
-      <c r="D9" s="21" t="s">
+      <c r="D9" s="41" t="s">
         <v>63</v>
       </c>
-      <c r="E9" s="21" t="s">
+      <c r="E9" s="41" t="s">
         <v>65</v>
       </c>
-      <c r="F9" s="21">
+      <c r="F9" s="41">
         <v>1</v>
       </c>
-      <c r="G9" s="21" t="s">
+      <c r="G9" s="41" t="s">
         <v>45</v>
       </c>
-      <c r="H9" s="24" t="s">
+      <c r="H9" s="44" t="s">
         <v>143</v>
       </c>
-      <c r="I9" s="42" t="s">
+      <c r="I9" s="50" t="s">
         <v>81</v>
       </c>
-      <c r="J9" s="37"/>
+      <c r="J9" s="21"/>
       <c r="K9" s="13">
         <v>1</v>
       </c>
@@ -2316,21 +2250,21 @@
         <v>46</v>
       </c>
       <c r="P9" s="13"/>
-      <c r="Q9" s="47"/>
-      <c r="R9" s="18" t="s">
+      <c r="Q9" s="25"/>
+      <c r="R9" s="35" t="s">
         <v>90</v>
       </c>
     </row>
     <row r="10" spans="1:19" ht="24" x14ac:dyDescent="0.2">
-      <c r="A10" s="28"/>
-      <c r="B10" s="22"/>
-      <c r="C10" s="22"/>
-      <c r="D10" s="22"/>
-      <c r="E10" s="22"/>
-      <c r="F10" s="22"/>
-      <c r="G10" s="22"/>
-      <c r="H10" s="25"/>
-      <c r="I10" s="42"/>
+      <c r="A10" s="39"/>
+      <c r="B10" s="42"/>
+      <c r="C10" s="42"/>
+      <c r="D10" s="42"/>
+      <c r="E10" s="42"/>
+      <c r="F10" s="42"/>
+      <c r="G10" s="42"/>
+      <c r="H10" s="45"/>
+      <c r="I10" s="50"/>
       <c r="K10" s="4">
         <v>2</v>
       </c>
@@ -2346,18 +2280,18 @@
       <c r="O10" s="4" t="s">
         <v>46</v>
       </c>
-      <c r="R10" s="19"/>
+      <c r="R10" s="36"/>
     </row>
     <row r="11" spans="1:19" ht="24" x14ac:dyDescent="0.2">
-      <c r="A11" s="28"/>
-      <c r="B11" s="22"/>
-      <c r="C11" s="22"/>
-      <c r="D11" s="22"/>
-      <c r="E11" s="22"/>
-      <c r="F11" s="22"/>
-      <c r="G11" s="22"/>
-      <c r="H11" s="25"/>
-      <c r="I11" s="42"/>
+      <c r="A11" s="39"/>
+      <c r="B11" s="42"/>
+      <c r="C11" s="42"/>
+      <c r="D11" s="42"/>
+      <c r="E11" s="42"/>
+      <c r="F11" s="42"/>
+      <c r="G11" s="42"/>
+      <c r="H11" s="45"/>
+      <c r="I11" s="50"/>
       <c r="K11" s="4">
         <v>3</v>
       </c>
@@ -2373,18 +2307,18 @@
       <c r="O11" s="4" t="s">
         <v>46</v>
       </c>
-      <c r="R11" s="19"/>
+      <c r="R11" s="36"/>
     </row>
     <row r="12" spans="1:19" ht="31.5" x14ac:dyDescent="0.2">
-      <c r="A12" s="28"/>
-      <c r="B12" s="22"/>
-      <c r="C12" s="22"/>
-      <c r="D12" s="22"/>
-      <c r="E12" s="22"/>
-      <c r="F12" s="22"/>
-      <c r="G12" s="22"/>
-      <c r="H12" s="25"/>
-      <c r="I12" s="42"/>
+      <c r="A12" s="39"/>
+      <c r="B12" s="42"/>
+      <c r="C12" s="42"/>
+      <c r="D12" s="42"/>
+      <c r="E12" s="42"/>
+      <c r="F12" s="42"/>
+      <c r="G12" s="42"/>
+      <c r="H12" s="45"/>
+      <c r="I12" s="50"/>
       <c r="K12" s="4">
         <v>4</v>
       </c>
@@ -2403,21 +2337,21 @@
       <c r="P12" s="4" t="s">
         <v>152</v>
       </c>
-      <c r="Q12" s="48" t="s">
+      <c r="Q12" s="26" t="s">
         <v>151</v>
       </c>
-      <c r="R12" s="19"/>
+      <c r="R12" s="36"/>
     </row>
     <row r="13" spans="1:19" ht="24" x14ac:dyDescent="0.2">
-      <c r="A13" s="28"/>
-      <c r="B13" s="22"/>
-      <c r="C13" s="22"/>
-      <c r="D13" s="22"/>
-      <c r="E13" s="22"/>
-      <c r="F13" s="22"/>
-      <c r="G13" s="22"/>
-      <c r="H13" s="25"/>
-      <c r="I13" s="42"/>
+      <c r="A13" s="39"/>
+      <c r="B13" s="42"/>
+      <c r="C13" s="42"/>
+      <c r="D13" s="42"/>
+      <c r="E13" s="42"/>
+      <c r="F13" s="42"/>
+      <c r="G13" s="42"/>
+      <c r="H13" s="45"/>
+      <c r="I13" s="50"/>
       <c r="K13" s="4">
         <v>5</v>
       </c>
@@ -2433,18 +2367,18 @@
       <c r="O13" s="4" t="s">
         <v>46</v>
       </c>
-      <c r="R13" s="19"/>
+      <c r="R13" s="36"/>
     </row>
     <row r="14" spans="1:19" ht="36" x14ac:dyDescent="0.2">
-      <c r="A14" s="28"/>
-      <c r="B14" s="22"/>
-      <c r="C14" s="22"/>
-      <c r="D14" s="22"/>
-      <c r="E14" s="22"/>
-      <c r="F14" s="22"/>
-      <c r="G14" s="22"/>
-      <c r="H14" s="25"/>
-      <c r="I14" s="42"/>
+      <c r="A14" s="39"/>
+      <c r="B14" s="42"/>
+      <c r="C14" s="42"/>
+      <c r="D14" s="42"/>
+      <c r="E14" s="42"/>
+      <c r="F14" s="42"/>
+      <c r="G14" s="42"/>
+      <c r="H14" s="45"/>
+      <c r="I14" s="50"/>
       <c r="K14" s="4">
         <v>6</v>
       </c>
@@ -2460,18 +2394,18 @@
       <c r="O14" s="4" t="s">
         <v>46</v>
       </c>
-      <c r="R14" s="19"/>
+      <c r="R14" s="36"/>
     </row>
     <row r="15" spans="1:19" ht="24" x14ac:dyDescent="0.2">
-      <c r="A15" s="28"/>
-      <c r="B15" s="22"/>
-      <c r="C15" s="22"/>
-      <c r="D15" s="22"/>
-      <c r="E15" s="22"/>
-      <c r="F15" s="22"/>
-      <c r="G15" s="22"/>
-      <c r="H15" s="25"/>
-      <c r="I15" s="42"/>
+      <c r="A15" s="39"/>
+      <c r="B15" s="42"/>
+      <c r="C15" s="42"/>
+      <c r="D15" s="42"/>
+      <c r="E15" s="42"/>
+      <c r="F15" s="42"/>
+      <c r="G15" s="42"/>
+      <c r="H15" s="45"/>
+      <c r="I15" s="50"/>
       <c r="K15" s="4">
         <v>7</v>
       </c>
@@ -2487,19 +2421,19 @@
       <c r="O15" s="4" t="s">
         <v>46</v>
       </c>
-      <c r="R15" s="19"/>
+      <c r="R15" s="36"/>
     </row>
     <row r="16" spans="1:19" ht="24.75" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="29"/>
-      <c r="B16" s="23"/>
-      <c r="C16" s="23"/>
-      <c r="D16" s="23"/>
-      <c r="E16" s="23"/>
-      <c r="F16" s="23"/>
-      <c r="G16" s="23"/>
-      <c r="H16" s="26"/>
-      <c r="I16" s="42"/>
-      <c r="J16" s="41"/>
+      <c r="A16" s="40"/>
+      <c r="B16" s="43"/>
+      <c r="C16" s="43"/>
+      <c r="D16" s="43"/>
+      <c r="E16" s="43"/>
+      <c r="F16" s="43"/>
+      <c r="G16" s="43"/>
+      <c r="H16" s="46"/>
+      <c r="I16" s="50"/>
+      <c r="J16" s="23"/>
       <c r="K16" s="4">
         <v>8</v>
       </c>
@@ -2516,38 +2450,38 @@
         <v>46</v>
       </c>
       <c r="P16" s="14"/>
-      <c r="Q16" s="49"/>
-      <c r="R16" s="20"/>
+      <c r="Q16" s="27"/>
+      <c r="R16" s="37"/>
     </row>
     <row r="17" spans="1:18" ht="24" x14ac:dyDescent="0.2">
-      <c r="A17" s="27">
+      <c r="A17" s="38">
         <v>3</v>
       </c>
-      <c r="B17" s="21" t="s">
-        <v>46</v>
-      </c>
-      <c r="C17" s="21" t="s">
+      <c r="B17" s="41" t="s">
+        <v>46</v>
+      </c>
+      <c r="C17" s="41" t="s">
         <v>49</v>
       </c>
-      <c r="D17" s="21" t="s">
+      <c r="D17" s="41" t="s">
         <v>69</v>
       </c>
-      <c r="E17" s="21" t="s">
+      <c r="E17" s="41" t="s">
         <v>70</v>
       </c>
-      <c r="F17" s="21">
+      <c r="F17" s="41">
         <v>1</v>
       </c>
-      <c r="G17" s="21" t="s">
+      <c r="G17" s="41" t="s">
         <v>45</v>
       </c>
-      <c r="H17" s="24" t="s">
+      <c r="H17" s="44" t="s">
         <v>144</v>
       </c>
-      <c r="I17" s="36" t="s">
+      <c r="I17" s="47" t="s">
         <v>81</v>
       </c>
-      <c r="J17" s="37"/>
+      <c r="J17" s="21"/>
       <c r="K17" s="13">
         <v>1</v>
       </c>
@@ -2564,19 +2498,19 @@
         <v>46</v>
       </c>
       <c r="P17" s="13"/>
-      <c r="Q17" s="50"/>
-      <c r="R17" s="18"/>
+      <c r="Q17" s="28"/>
+      <c r="R17" s="35"/>
     </row>
     <row r="18" spans="1:18" ht="24" x14ac:dyDescent="0.2">
-      <c r="A18" s="28"/>
-      <c r="B18" s="22"/>
-      <c r="C18" s="22"/>
-      <c r="D18" s="22"/>
-      <c r="E18" s="22"/>
-      <c r="F18" s="22"/>
-      <c r="G18" s="22"/>
-      <c r="H18" s="25"/>
-      <c r="I18" s="38"/>
+      <c r="A18" s="39"/>
+      <c r="B18" s="42"/>
+      <c r="C18" s="42"/>
+      <c r="D18" s="42"/>
+      <c r="E18" s="42"/>
+      <c r="F18" s="42"/>
+      <c r="G18" s="42"/>
+      <c r="H18" s="45"/>
+      <c r="I18" s="48"/>
       <c r="K18" s="4">
         <v>2</v>
       </c>
@@ -2592,19 +2526,19 @@
       <c r="O18" s="4" t="s">
         <v>46</v>
       </c>
-      <c r="Q18" s="51"/>
-      <c r="R18" s="19"/>
+      <c r="Q18" s="29"/>
+      <c r="R18" s="36"/>
     </row>
     <row r="19" spans="1:18" ht="24" x14ac:dyDescent="0.2">
-      <c r="A19" s="28"/>
-      <c r="B19" s="22"/>
-      <c r="C19" s="22"/>
-      <c r="D19" s="22"/>
-      <c r="E19" s="22"/>
-      <c r="F19" s="22"/>
-      <c r="G19" s="22"/>
-      <c r="H19" s="25"/>
-      <c r="I19" s="38"/>
+      <c r="A19" s="39"/>
+      <c r="B19" s="42"/>
+      <c r="C19" s="42"/>
+      <c r="D19" s="42"/>
+      <c r="E19" s="42"/>
+      <c r="F19" s="42"/>
+      <c r="G19" s="42"/>
+      <c r="H19" s="45"/>
+      <c r="I19" s="48"/>
       <c r="K19" s="4">
         <v>3</v>
       </c>
@@ -2620,19 +2554,19 @@
       <c r="O19" s="4" t="s">
         <v>46</v>
       </c>
-      <c r="Q19" s="51"/>
-      <c r="R19" s="19"/>
+      <c r="Q19" s="29"/>
+      <c r="R19" s="36"/>
     </row>
     <row r="20" spans="1:18" ht="12" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A20" s="28"/>
-      <c r="B20" s="22"/>
-      <c r="C20" s="22"/>
-      <c r="D20" s="22"/>
-      <c r="E20" s="22"/>
-      <c r="F20" s="22"/>
-      <c r="G20" s="22"/>
-      <c r="H20" s="25"/>
-      <c r="I20" s="38"/>
+      <c r="A20" s="39"/>
+      <c r="B20" s="42"/>
+      <c r="C20" s="42"/>
+      <c r="D20" s="42"/>
+      <c r="E20" s="42"/>
+      <c r="F20" s="42"/>
+      <c r="G20" s="42"/>
+      <c r="H20" s="45"/>
+      <c r="I20" s="48"/>
       <c r="K20" s="4">
         <v>4</v>
       </c>
@@ -2648,19 +2582,19 @@
       <c r="O20" s="4" t="s">
         <v>46</v>
       </c>
-      <c r="Q20" s="51"/>
-      <c r="R20" s="19"/>
+      <c r="Q20" s="29"/>
+      <c r="R20" s="36"/>
     </row>
     <row r="21" spans="1:18" ht="36" x14ac:dyDescent="0.2">
-      <c r="A21" s="28"/>
-      <c r="B21" s="22"/>
-      <c r="C21" s="22"/>
-      <c r="D21" s="22"/>
-      <c r="E21" s="22"/>
-      <c r="F21" s="22"/>
-      <c r="G21" s="22"/>
-      <c r="H21" s="25"/>
-      <c r="I21" s="38"/>
+      <c r="A21" s="39"/>
+      <c r="B21" s="42"/>
+      <c r="C21" s="42"/>
+      <c r="D21" s="42"/>
+      <c r="E21" s="42"/>
+      <c r="F21" s="42"/>
+      <c r="G21" s="42"/>
+      <c r="H21" s="45"/>
+      <c r="I21" s="48"/>
       <c r="K21" s="4">
         <v>5</v>
       </c>
@@ -2676,19 +2610,19 @@
       <c r="O21" s="4" t="s">
         <v>46</v>
       </c>
-      <c r="Q21" s="51"/>
-      <c r="R21" s="19"/>
+      <c r="Q21" s="29"/>
+      <c r="R21" s="36"/>
     </row>
     <row r="22" spans="1:18" ht="24" x14ac:dyDescent="0.2">
-      <c r="A22" s="28"/>
-      <c r="B22" s="22"/>
-      <c r="C22" s="22"/>
-      <c r="D22" s="22"/>
-      <c r="E22" s="22"/>
-      <c r="F22" s="22"/>
-      <c r="G22" s="22"/>
-      <c r="H22" s="25"/>
-      <c r="I22" s="38"/>
+      <c r="A22" s="39"/>
+      <c r="B22" s="42"/>
+      <c r="C22" s="42"/>
+      <c r="D22" s="42"/>
+      <c r="E22" s="42"/>
+      <c r="F22" s="42"/>
+      <c r="G22" s="42"/>
+      <c r="H22" s="45"/>
+      <c r="I22" s="48"/>
       <c r="K22" s="4">
         <v>6</v>
       </c>
@@ -2704,19 +2638,19 @@
       <c r="O22" s="4" t="s">
         <v>46</v>
       </c>
-      <c r="Q22" s="51"/>
-      <c r="R22" s="19"/>
+      <c r="Q22" s="29"/>
+      <c r="R22" s="36"/>
     </row>
     <row r="23" spans="1:18" ht="36" x14ac:dyDescent="0.2">
-      <c r="A23" s="28"/>
-      <c r="B23" s="22"/>
-      <c r="C23" s="22"/>
-      <c r="D23" s="22"/>
-      <c r="E23" s="22"/>
-      <c r="F23" s="22"/>
-      <c r="G23" s="22"/>
-      <c r="H23" s="25"/>
-      <c r="I23" s="38"/>
+      <c r="A23" s="39"/>
+      <c r="B23" s="42"/>
+      <c r="C23" s="42"/>
+      <c r="D23" s="42"/>
+      <c r="E23" s="42"/>
+      <c r="F23" s="42"/>
+      <c r="G23" s="42"/>
+      <c r="H23" s="45"/>
+      <c r="I23" s="48"/>
       <c r="K23" s="4">
         <v>7</v>
       </c>
@@ -2732,19 +2666,19 @@
       <c r="O23" s="4" t="s">
         <v>46</v>
       </c>
-      <c r="Q23" s="51"/>
-      <c r="R23" s="19"/>
+      <c r="Q23" s="29"/>
+      <c r="R23" s="36"/>
     </row>
     <row r="24" spans="1:18" ht="24" x14ac:dyDescent="0.2">
-      <c r="A24" s="28"/>
-      <c r="B24" s="22"/>
-      <c r="C24" s="22"/>
-      <c r="D24" s="22"/>
-      <c r="E24" s="22"/>
-      <c r="F24" s="22"/>
-      <c r="G24" s="22"/>
-      <c r="H24" s="25"/>
-      <c r="I24" s="38"/>
+      <c r="A24" s="39"/>
+      <c r="B24" s="42"/>
+      <c r="C24" s="42"/>
+      <c r="D24" s="42"/>
+      <c r="E24" s="42"/>
+      <c r="F24" s="42"/>
+      <c r="G24" s="42"/>
+      <c r="H24" s="45"/>
+      <c r="I24" s="48"/>
       <c r="L24" s="4" t="s">
         <v>74</v>
       </c>
@@ -2757,20 +2691,20 @@
       <c r="O24" s="4" t="s">
         <v>46</v>
       </c>
-      <c r="Q24" s="51"/>
-      <c r="R24" s="19"/>
+      <c r="Q24" s="29"/>
+      <c r="R24" s="36"/>
     </row>
     <row r="25" spans="1:18" ht="36.75" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A25" s="29"/>
-      <c r="B25" s="23"/>
-      <c r="C25" s="23"/>
-      <c r="D25" s="23"/>
-      <c r="E25" s="23"/>
-      <c r="F25" s="23"/>
-      <c r="G25" s="23"/>
-      <c r="H25" s="26"/>
-      <c r="I25" s="40"/>
-      <c r="J25" s="41"/>
+      <c r="A25" s="40"/>
+      <c r="B25" s="43"/>
+      <c r="C25" s="43"/>
+      <c r="D25" s="43"/>
+      <c r="E25" s="43"/>
+      <c r="F25" s="43"/>
+      <c r="G25" s="43"/>
+      <c r="H25" s="46"/>
+      <c r="I25" s="49"/>
+      <c r="J25" s="23"/>
       <c r="K25" s="4">
         <v>8</v>
       </c>
@@ -2787,38 +2721,38 @@
         <v>46</v>
       </c>
       <c r="P25" s="14"/>
-      <c r="Q25" s="52"/>
-      <c r="R25" s="20"/>
+      <c r="Q25" s="30"/>
+      <c r="R25" s="37"/>
     </row>
     <row r="26" spans="1:18" ht="48" x14ac:dyDescent="0.2">
-      <c r="A26" s="27">
+      <c r="A26" s="38">
         <v>4</v>
       </c>
-      <c r="B26" s="21" t="s">
+      <c r="B26" s="41" t="s">
         <v>89</v>
       </c>
-      <c r="C26" s="21" t="s">
+      <c r="C26" s="41" t="s">
         <v>49</v>
       </c>
-      <c r="D26" s="21" t="s">
+      <c r="D26" s="41" t="s">
         <v>123</v>
       </c>
-      <c r="E26" s="21" t="s">
+      <c r="E26" s="41" t="s">
         <v>75</v>
       </c>
-      <c r="F26" s="21">
+      <c r="F26" s="41">
         <v>1</v>
       </c>
-      <c r="G26" s="21" t="s">
+      <c r="G26" s="41" t="s">
         <v>45</v>
       </c>
-      <c r="H26" s="24" t="s">
+      <c r="H26" s="44" t="s">
         <v>145</v>
       </c>
-      <c r="I26" s="36" t="s">
+      <c r="I26" s="47" t="s">
         <v>81</v>
       </c>
-      <c r="J26" s="37"/>
+      <c r="J26" s="21"/>
       <c r="K26" s="13">
         <v>1</v>
       </c>
@@ -2837,21 +2771,21 @@
       <c r="P26" s="13" t="s">
         <v>125</v>
       </c>
-      <c r="Q26" s="47" t="s">
+      <c r="Q26" s="25" t="s">
         <v>150</v>
       </c>
-      <c r="R26" s="18"/>
+      <c r="R26" s="35"/>
     </row>
     <row r="27" spans="1:18" ht="36" x14ac:dyDescent="0.2">
-      <c r="A27" s="28"/>
-      <c r="B27" s="22"/>
-      <c r="C27" s="22"/>
-      <c r="D27" s="22"/>
-      <c r="E27" s="22"/>
-      <c r="F27" s="22"/>
-      <c r="G27" s="22"/>
-      <c r="H27" s="25"/>
-      <c r="I27" s="38"/>
+      <c r="A27" s="39"/>
+      <c r="B27" s="42"/>
+      <c r="C27" s="42"/>
+      <c r="D27" s="42"/>
+      <c r="E27" s="42"/>
+      <c r="F27" s="42"/>
+      <c r="G27" s="42"/>
+      <c r="H27" s="45"/>
+      <c r="I27" s="48"/>
       <c r="K27" s="4">
         <v>2</v>
       </c>
@@ -2867,18 +2801,18 @@
       <c r="O27" s="4" t="s">
         <v>46</v>
       </c>
-      <c r="R27" s="19"/>
+      <c r="R27" s="36"/>
     </row>
     <row r="28" spans="1:18" ht="24" x14ac:dyDescent="0.2">
-      <c r="A28" s="28"/>
-      <c r="B28" s="22"/>
-      <c r="C28" s="22"/>
-      <c r="D28" s="22"/>
-      <c r="E28" s="22"/>
-      <c r="F28" s="22"/>
-      <c r="G28" s="22"/>
-      <c r="H28" s="25"/>
-      <c r="I28" s="38"/>
+      <c r="A28" s="39"/>
+      <c r="B28" s="42"/>
+      <c r="C28" s="42"/>
+      <c r="D28" s="42"/>
+      <c r="E28" s="42"/>
+      <c r="F28" s="42"/>
+      <c r="G28" s="42"/>
+      <c r="H28" s="45"/>
+      <c r="I28" s="48"/>
       <c r="K28" s="4">
         <v>3</v>
       </c>
@@ -2894,18 +2828,18 @@
       <c r="O28" s="4" t="s">
         <v>46</v>
       </c>
-      <c r="R28" s="19"/>
+      <c r="R28" s="36"/>
     </row>
     <row r="29" spans="1:18" ht="36" x14ac:dyDescent="0.2">
-      <c r="A29" s="28"/>
-      <c r="B29" s="22"/>
-      <c r="C29" s="22"/>
-      <c r="D29" s="22"/>
-      <c r="E29" s="22"/>
-      <c r="F29" s="22"/>
-      <c r="G29" s="22"/>
-      <c r="H29" s="25"/>
-      <c r="I29" s="38"/>
+      <c r="A29" s="39"/>
+      <c r="B29" s="42"/>
+      <c r="C29" s="42"/>
+      <c r="D29" s="42"/>
+      <c r="E29" s="42"/>
+      <c r="F29" s="42"/>
+      <c r="G29" s="42"/>
+      <c r="H29" s="45"/>
+      <c r="I29" s="48"/>
       <c r="K29" s="4">
         <v>4</v>
       </c>
@@ -2921,18 +2855,18 @@
       <c r="O29" s="4" t="s">
         <v>46</v>
       </c>
-      <c r="R29" s="19"/>
+      <c r="R29" s="36"/>
     </row>
     <row r="30" spans="1:18" ht="36" x14ac:dyDescent="0.2">
-      <c r="A30" s="28"/>
-      <c r="B30" s="22"/>
-      <c r="C30" s="22"/>
-      <c r="D30" s="22"/>
-      <c r="E30" s="22"/>
-      <c r="F30" s="22"/>
-      <c r="G30" s="22"/>
-      <c r="H30" s="25"/>
-      <c r="I30" s="38"/>
+      <c r="A30" s="39"/>
+      <c r="B30" s="42"/>
+      <c r="C30" s="42"/>
+      <c r="D30" s="42"/>
+      <c r="E30" s="42"/>
+      <c r="F30" s="42"/>
+      <c r="G30" s="42"/>
+      <c r="H30" s="45"/>
+      <c r="I30" s="48"/>
       <c r="K30" s="4">
         <v>5</v>
       </c>
@@ -2948,18 +2882,18 @@
       <c r="O30" s="4" t="s">
         <v>46</v>
       </c>
-      <c r="R30" s="19"/>
+      <c r="R30" s="36"/>
     </row>
     <row r="31" spans="1:18" ht="36" x14ac:dyDescent="0.2">
-      <c r="A31" s="28"/>
-      <c r="B31" s="22"/>
-      <c r="C31" s="22"/>
-      <c r="D31" s="22"/>
-      <c r="E31" s="22"/>
-      <c r="F31" s="22"/>
-      <c r="G31" s="22"/>
-      <c r="H31" s="25"/>
-      <c r="I31" s="38"/>
+      <c r="A31" s="39"/>
+      <c r="B31" s="42"/>
+      <c r="C31" s="42"/>
+      <c r="D31" s="42"/>
+      <c r="E31" s="42"/>
+      <c r="F31" s="42"/>
+      <c r="G31" s="42"/>
+      <c r="H31" s="45"/>
+      <c r="I31" s="48"/>
       <c r="K31" s="4">
         <v>6</v>
       </c>
@@ -2975,18 +2909,18 @@
       <c r="O31" s="4" t="s">
         <v>46</v>
       </c>
-      <c r="R31" s="19"/>
+      <c r="R31" s="36"/>
     </row>
     <row r="32" spans="1:18" ht="24" x14ac:dyDescent="0.2">
-      <c r="A32" s="28"/>
-      <c r="B32" s="22"/>
-      <c r="C32" s="22"/>
-      <c r="D32" s="22"/>
-      <c r="E32" s="22"/>
-      <c r="F32" s="22"/>
-      <c r="G32" s="22"/>
-      <c r="H32" s="25"/>
-      <c r="I32" s="38"/>
+      <c r="A32" s="39"/>
+      <c r="B32" s="42"/>
+      <c r="C32" s="42"/>
+      <c r="D32" s="42"/>
+      <c r="E32" s="42"/>
+      <c r="F32" s="42"/>
+      <c r="G32" s="42"/>
+      <c r="H32" s="45"/>
+      <c r="I32" s="48"/>
       <c r="K32" s="4">
         <v>7</v>
       </c>
@@ -3002,18 +2936,18 @@
       <c r="O32" s="4" t="s">
         <v>46</v>
       </c>
-      <c r="R32" s="19"/>
+      <c r="R32" s="36"/>
     </row>
     <row r="33" spans="1:18" x14ac:dyDescent="0.2">
-      <c r="A33" s="28"/>
-      <c r="B33" s="22"/>
-      <c r="C33" s="22"/>
-      <c r="D33" s="22"/>
-      <c r="E33" s="22"/>
-      <c r="F33" s="22"/>
-      <c r="G33" s="22"/>
-      <c r="H33" s="25"/>
-      <c r="I33" s="38"/>
+      <c r="A33" s="39"/>
+      <c r="B33" s="42"/>
+      <c r="C33" s="42"/>
+      <c r="D33" s="42"/>
+      <c r="E33" s="42"/>
+      <c r="F33" s="42"/>
+      <c r="G33" s="42"/>
+      <c r="H33" s="45"/>
+      <c r="I33" s="48"/>
       <c r="K33" s="4">
         <v>8</v>
       </c>
@@ -3029,18 +2963,18 @@
       <c r="O33" s="4" t="s">
         <v>46</v>
       </c>
-      <c r="R33" s="19"/>
+      <c r="R33" s="36"/>
     </row>
     <row r="34" spans="1:18" ht="24.75" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A34" s="28"/>
-      <c r="B34" s="22"/>
-      <c r="C34" s="22"/>
-      <c r="D34" s="22"/>
-      <c r="E34" s="22"/>
-      <c r="F34" s="22"/>
-      <c r="G34" s="22"/>
-      <c r="H34" s="25"/>
-      <c r="I34" s="38"/>
+      <c r="A34" s="39"/>
+      <c r="B34" s="42"/>
+      <c r="C34" s="42"/>
+      <c r="D34" s="42"/>
+      <c r="E34" s="42"/>
+      <c r="F34" s="42"/>
+      <c r="G34" s="42"/>
+      <c r="H34" s="45"/>
+      <c r="I34" s="48"/>
       <c r="K34" s="4">
         <v>9</v>
       </c>
@@ -3056,37 +2990,37 @@
       <c r="O34" s="4" t="s">
         <v>46</v>
       </c>
-      <c r="R34" s="19"/>
+      <c r="R34" s="36"/>
     </row>
     <row r="35" spans="1:18" ht="12" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A35" s="27">
+      <c r="A35" s="38">
         <v>5</v>
       </c>
-      <c r="B35" s="21" t="s">
-        <v>46</v>
-      </c>
-      <c r="C35" s="21" t="s">
+      <c r="B35" s="41" t="s">
+        <v>46</v>
+      </c>
+      <c r="C35" s="41" t="s">
         <v>49</v>
       </c>
-      <c r="D35" s="21" t="s">
+      <c r="D35" s="41" t="s">
         <v>80</v>
       </c>
-      <c r="E35" s="21" t="s">
+      <c r="E35" s="41" t="s">
         <v>110</v>
       </c>
-      <c r="F35" s="21">
+      <c r="F35" s="41">
         <v>1</v>
       </c>
-      <c r="G35" s="21" t="s">
+      <c r="G35" s="41" t="s">
         <v>45</v>
       </c>
-      <c r="H35" s="24" t="s">
+      <c r="H35" s="44" t="s">
         <v>146</v>
       </c>
-      <c r="I35" s="36" t="s">
+      <c r="I35" s="47" t="s">
         <v>81</v>
       </c>
-      <c r="J35" s="37"/>
+      <c r="J35" s="21"/>
       <c r="K35" s="13">
         <v>1</v>
       </c>
@@ -3103,19 +3037,19 @@
         <v>46</v>
       </c>
       <c r="P35" s="13"/>
-      <c r="Q35" s="50"/>
-      <c r="R35" s="18"/>
+      <c r="Q35" s="28"/>
+      <c r="R35" s="35"/>
     </row>
     <row r="36" spans="1:18" ht="24" x14ac:dyDescent="0.2">
-      <c r="A36" s="28"/>
-      <c r="B36" s="22"/>
-      <c r="C36" s="22"/>
-      <c r="D36" s="22"/>
-      <c r="E36" s="22"/>
-      <c r="F36" s="22"/>
-      <c r="G36" s="22"/>
-      <c r="H36" s="25"/>
-      <c r="I36" s="38"/>
+      <c r="A36" s="39"/>
+      <c r="B36" s="42"/>
+      <c r="C36" s="42"/>
+      <c r="D36" s="42"/>
+      <c r="E36" s="42"/>
+      <c r="F36" s="42"/>
+      <c r="G36" s="42"/>
+      <c r="H36" s="45"/>
+      <c r="I36" s="48"/>
       <c r="K36" s="4">
         <v>2</v>
       </c>
@@ -3131,19 +3065,19 @@
       <c r="O36" s="4" t="s">
         <v>46</v>
       </c>
-      <c r="Q36" s="51"/>
-      <c r="R36" s="19"/>
+      <c r="Q36" s="29"/>
+      <c r="R36" s="36"/>
     </row>
     <row r="37" spans="1:18" ht="12" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A37" s="28"/>
-      <c r="B37" s="22"/>
-      <c r="C37" s="22"/>
-      <c r="D37" s="22"/>
-      <c r="E37" s="22"/>
-      <c r="F37" s="22"/>
-      <c r="G37" s="22"/>
-      <c r="H37" s="25"/>
-      <c r="I37" s="38"/>
+      <c r="A37" s="39"/>
+      <c r="B37" s="42"/>
+      <c r="C37" s="42"/>
+      <c r="D37" s="42"/>
+      <c r="E37" s="42"/>
+      <c r="F37" s="42"/>
+      <c r="G37" s="42"/>
+      <c r="H37" s="45"/>
+      <c r="I37" s="48"/>
       <c r="K37" s="4">
         <v>4</v>
       </c>
@@ -3159,19 +3093,19 @@
       <c r="O37" s="4" t="s">
         <v>46</v>
       </c>
-      <c r="Q37" s="51"/>
-      <c r="R37" s="19"/>
+      <c r="Q37" s="29"/>
+      <c r="R37" s="36"/>
     </row>
     <row r="38" spans="1:18" ht="24" x14ac:dyDescent="0.2">
-      <c r="A38" s="28"/>
-      <c r="B38" s="22"/>
-      <c r="C38" s="22"/>
-      <c r="D38" s="22"/>
-      <c r="E38" s="22"/>
-      <c r="F38" s="22"/>
-      <c r="G38" s="22"/>
-      <c r="H38" s="25"/>
-      <c r="I38" s="38"/>
+      <c r="A38" s="39"/>
+      <c r="B38" s="42"/>
+      <c r="C38" s="42"/>
+      <c r="D38" s="42"/>
+      <c r="E38" s="42"/>
+      <c r="F38" s="42"/>
+      <c r="G38" s="42"/>
+      <c r="H38" s="45"/>
+      <c r="I38" s="48"/>
       <c r="K38" s="4">
         <v>5</v>
       </c>
@@ -3187,19 +3121,19 @@
       <c r="O38" s="4" t="s">
         <v>46</v>
       </c>
-      <c r="Q38" s="51"/>
-      <c r="R38" s="19"/>
+      <c r="Q38" s="29"/>
+      <c r="R38" s="36"/>
     </row>
     <row r="39" spans="1:18" ht="12" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A39" s="28"/>
-      <c r="B39" s="22"/>
-      <c r="C39" s="22"/>
-      <c r="D39" s="22"/>
-      <c r="E39" s="22"/>
-      <c r="F39" s="22"/>
-      <c r="G39" s="22"/>
-      <c r="H39" s="25"/>
-      <c r="I39" s="38"/>
+      <c r="A39" s="39"/>
+      <c r="B39" s="42"/>
+      <c r="C39" s="42"/>
+      <c r="D39" s="42"/>
+      <c r="E39" s="42"/>
+      <c r="F39" s="42"/>
+      <c r="G39" s="42"/>
+      <c r="H39" s="45"/>
+      <c r="I39" s="48"/>
       <c r="K39" s="4">
         <v>7</v>
       </c>
@@ -3215,19 +3149,19 @@
       <c r="O39" s="4" t="s">
         <v>46</v>
       </c>
-      <c r="Q39" s="51"/>
-      <c r="R39" s="19"/>
+      <c r="Q39" s="29"/>
+      <c r="R39" s="36"/>
     </row>
     <row r="40" spans="1:18" ht="24.75" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A40" s="28"/>
-      <c r="B40" s="22"/>
-      <c r="C40" s="22"/>
-      <c r="D40" s="22"/>
-      <c r="E40" s="22"/>
-      <c r="F40" s="22"/>
-      <c r="G40" s="22"/>
-      <c r="H40" s="25"/>
-      <c r="I40" s="38"/>
+      <c r="A40" s="39"/>
+      <c r="B40" s="42"/>
+      <c r="C40" s="42"/>
+      <c r="D40" s="42"/>
+      <c r="E40" s="42"/>
+      <c r="F40" s="42"/>
+      <c r="G40" s="42"/>
+      <c r="H40" s="45"/>
+      <c r="I40" s="48"/>
       <c r="K40" s="4">
         <v>8</v>
       </c>
@@ -3243,38 +3177,38 @@
       <c r="O40" s="4" t="s">
         <v>46</v>
       </c>
-      <c r="Q40" s="51"/>
-      <c r="R40" s="19"/>
+      <c r="Q40" s="29"/>
+      <c r="R40" s="36"/>
     </row>
     <row r="41" spans="1:18" ht="36" x14ac:dyDescent="0.2">
-      <c r="A41" s="27">
+      <c r="A41" s="38">
         <v>6</v>
       </c>
-      <c r="B41" s="21" t="s">
-        <v>46</v>
-      </c>
-      <c r="C41" s="21" t="s">
+      <c r="B41" s="41" t="s">
+        <v>46</v>
+      </c>
+      <c r="C41" s="41" t="s">
         <v>49</v>
       </c>
-      <c r="D41" s="21" t="s">
+      <c r="D41" s="41" t="s">
         <v>115</v>
       </c>
-      <c r="E41" s="21" t="s">
+      <c r="E41" s="41" t="s">
         <v>116</v>
       </c>
-      <c r="F41" s="21">
+      <c r="F41" s="41">
         <v>1</v>
       </c>
-      <c r="G41" s="21" t="s">
+      <c r="G41" s="41" t="s">
         <v>45</v>
       </c>
-      <c r="H41" s="24" t="s">
+      <c r="H41" s="44" t="s">
         <v>147</v>
       </c>
-      <c r="I41" s="36" t="s">
+      <c r="I41" s="47" t="s">
         <v>81</v>
       </c>
-      <c r="J41" s="37"/>
+      <c r="J41" s="21"/>
       <c r="K41" s="13">
         <v>1</v>
       </c>
@@ -3291,19 +3225,19 @@
         <v>46</v>
       </c>
       <c r="P41" s="13"/>
-      <c r="Q41" s="50"/>
-      <c r="R41" s="18"/>
+      <c r="Q41" s="28"/>
+      <c r="R41" s="35"/>
     </row>
     <row r="42" spans="1:18" ht="36" x14ac:dyDescent="0.2">
-      <c r="A42" s="28"/>
-      <c r="B42" s="22"/>
-      <c r="C42" s="22"/>
-      <c r="D42" s="22"/>
-      <c r="E42" s="22"/>
-      <c r="F42" s="22"/>
-      <c r="G42" s="22"/>
-      <c r="H42" s="25"/>
-      <c r="I42" s="38"/>
+      <c r="A42" s="39"/>
+      <c r="B42" s="42"/>
+      <c r="C42" s="42"/>
+      <c r="D42" s="42"/>
+      <c r="E42" s="42"/>
+      <c r="F42" s="42"/>
+      <c r="G42" s="42"/>
+      <c r="H42" s="45"/>
+      <c r="I42" s="48"/>
       <c r="K42" s="4">
         <v>2</v>
       </c>
@@ -3319,20 +3253,20 @@
       <c r="O42" s="4" t="s">
         <v>46</v>
       </c>
-      <c r="Q42" s="51"/>
-      <c r="R42" s="19"/>
+      <c r="Q42" s="29"/>
+      <c r="R42" s="36"/>
     </row>
     <row r="43" spans="1:18" ht="24.75" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A43" s="29"/>
-      <c r="B43" s="23"/>
-      <c r="C43" s="23"/>
-      <c r="D43" s="23"/>
-      <c r="E43" s="23"/>
-      <c r="F43" s="23"/>
-      <c r="G43" s="23"/>
-      <c r="H43" s="26"/>
-      <c r="I43" s="40"/>
-      <c r="J43" s="41"/>
+      <c r="A43" s="40"/>
+      <c r="B43" s="43"/>
+      <c r="C43" s="43"/>
+      <c r="D43" s="43"/>
+      <c r="E43" s="43"/>
+      <c r="F43" s="43"/>
+      <c r="G43" s="43"/>
+      <c r="H43" s="46"/>
+      <c r="I43" s="49"/>
+      <c r="J43" s="23"/>
       <c r="K43" s="14">
         <v>4</v>
       </c>
@@ -3349,38 +3283,38 @@
         <v>46</v>
       </c>
       <c r="P43" s="14"/>
-      <c r="Q43" s="52"/>
-      <c r="R43" s="20"/>
+      <c r="Q43" s="30"/>
+      <c r="R43" s="37"/>
     </row>
     <row r="44" spans="1:18" ht="24" x14ac:dyDescent="0.2">
-      <c r="A44" s="27">
+      <c r="A44" s="38">
         <v>7</v>
       </c>
-      <c r="B44" s="21" t="s">
+      <c r="B44" s="41" t="s">
         <v>89</v>
       </c>
-      <c r="C44" s="21" t="s">
+      <c r="C44" s="41" t="s">
         <v>49</v>
       </c>
-      <c r="D44" s="21" t="s">
+      <c r="D44" s="41" t="s">
         <v>129</v>
       </c>
-      <c r="E44" s="21" t="s">
+      <c r="E44" s="41" t="s">
         <v>133</v>
       </c>
-      <c r="F44" s="21">
+      <c r="F44" s="41">
         <v>2</v>
       </c>
-      <c r="G44" s="21" t="s">
+      <c r="G44" s="41" t="s">
         <v>45</v>
       </c>
-      <c r="H44" s="24" t="s">
+      <c r="H44" s="44" t="s">
         <v>148</v>
       </c>
-      <c r="I44" s="43" t="s">
+      <c r="I44" s="51" t="s">
         <v>81</v>
       </c>
-      <c r="J44" s="37"/>
+      <c r="J44" s="21"/>
       <c r="K44" s="13">
         <v>1</v>
       </c>
@@ -3397,270 +3331,250 @@
         <v>46</v>
       </c>
       <c r="P44" s="13"/>
-      <c r="Q44" s="47"/>
-      <c r="R44" s="18" t="s">
+      <c r="Q44" s="25"/>
+      <c r="R44" s="35" t="s">
         <v>155</v>
       </c>
     </row>
     <row r="45" spans="1:18" ht="24" x14ac:dyDescent="0.2">
-      <c r="A45" s="28"/>
-      <c r="B45" s="53"/>
-      <c r="C45" s="53"/>
-      <c r="D45" s="53"/>
-      <c r="E45" s="53"/>
-      <c r="F45" s="53"/>
-      <c r="G45" s="53"/>
-      <c r="H45" s="54"/>
-      <c r="I45" s="44"/>
-      <c r="J45" s="55"/>
-      <c r="K45" s="30">
+      <c r="A45" s="39"/>
+      <c r="B45" s="42"/>
+      <c r="C45" s="42"/>
+      <c r="D45" s="42"/>
+      <c r="E45" s="42"/>
+      <c r="F45" s="42"/>
+      <c r="G45" s="42"/>
+      <c r="H45" s="45"/>
+      <c r="I45" s="52"/>
+      <c r="K45" s="4">
         <v>2</v>
       </c>
-      <c r="L45" s="30" t="s">
+      <c r="L45" s="4" t="s">
         <v>51</v>
       </c>
-      <c r="M45" s="30" t="s">
+      <c r="M45" s="4" t="s">
         <v>138</v>
       </c>
-      <c r="N45" s="30" t="s">
+      <c r="N45" s="4" t="s">
         <v>138</v>
       </c>
-      <c r="O45" s="30" t="s">
-        <v>46</v>
-      </c>
-      <c r="P45" s="30"/>
-      <c r="Q45" s="56"/>
-      <c r="R45" s="19"/>
+      <c r="O45" s="4" t="s">
+        <v>46</v>
+      </c>
+      <c r="R45" s="36"/>
     </row>
     <row r="46" spans="1:18" ht="24" x14ac:dyDescent="0.2">
-      <c r="A46" s="28"/>
-      <c r="B46" s="53"/>
-      <c r="C46" s="53"/>
-      <c r="D46" s="53"/>
-      <c r="E46" s="53"/>
-      <c r="F46" s="53"/>
-      <c r="G46" s="53"/>
-      <c r="H46" s="54"/>
-      <c r="I46" s="44"/>
-      <c r="J46" s="55"/>
-      <c r="K46" s="30">
+      <c r="A46" s="39"/>
+      <c r="B46" s="42"/>
+      <c r="C46" s="42"/>
+      <c r="D46" s="42"/>
+      <c r="E46" s="42"/>
+      <c r="F46" s="42"/>
+      <c r="G46" s="42"/>
+      <c r="H46" s="45"/>
+      <c r="I46" s="52"/>
+      <c r="K46" s="4">
         <v>3</v>
       </c>
-      <c r="L46" s="30" t="s">
+      <c r="L46" s="4" t="s">
         <v>130</v>
       </c>
-      <c r="M46" s="30" t="s">
+      <c r="M46" s="4" t="s">
         <v>135</v>
       </c>
-      <c r="N46" s="30" t="s">
+      <c r="N46" s="4" t="s">
         <v>135</v>
       </c>
-      <c r="O46" s="30" t="s">
-        <v>46</v>
-      </c>
-      <c r="P46" s="30"/>
-      <c r="Q46" s="56"/>
-      <c r="R46" s="19"/>
+      <c r="O46" s="4" t="s">
+        <v>46</v>
+      </c>
+      <c r="R46" s="36"/>
     </row>
     <row r="47" spans="1:18" ht="31.5" x14ac:dyDescent="0.2">
-      <c r="A47" s="28"/>
-      <c r="B47" s="53"/>
-      <c r="C47" s="53"/>
-      <c r="D47" s="53"/>
-      <c r="E47" s="53"/>
-      <c r="F47" s="53"/>
-      <c r="G47" s="53"/>
-      <c r="H47" s="54"/>
-      <c r="I47" s="44"/>
-      <c r="J47" s="55"/>
-      <c r="K47" s="30">
+      <c r="A47" s="39"/>
+      <c r="B47" s="42"/>
+      <c r="C47" s="42"/>
+      <c r="D47" s="42"/>
+      <c r="E47" s="42"/>
+      <c r="F47" s="42"/>
+      <c r="G47" s="42"/>
+      <c r="H47" s="45"/>
+      <c r="I47" s="52"/>
+      <c r="K47" s="4">
         <v>4</v>
       </c>
-      <c r="L47" s="30" t="s">
+      <c r="L47" s="4" t="s">
         <v>51</v>
       </c>
-      <c r="M47" s="30" t="s">
+      <c r="M47" s="4" t="s">
         <v>138</v>
       </c>
-      <c r="N47" s="30" t="s">
+      <c r="N47" s="4" t="s">
         <v>139</v>
       </c>
-      <c r="O47" s="30" t="s">
+      <c r="O47" s="4" t="s">
         <v>89</v>
       </c>
-      <c r="P47" s="57" t="s">
+      <c r="P47" s="31" t="s">
         <v>153</v>
       </c>
-      <c r="Q47" s="56" t="s">
+      <c r="Q47" s="26" t="s">
         <v>149</v>
       </c>
-      <c r="R47" s="19"/>
+      <c r="R47" s="36"/>
     </row>
     <row r="48" spans="1:18" ht="24" x14ac:dyDescent="0.2">
-      <c r="A48" s="28"/>
-      <c r="B48" s="53"/>
-      <c r="C48" s="53"/>
-      <c r="D48" s="53"/>
-      <c r="E48" s="53"/>
-      <c r="F48" s="53"/>
-      <c r="G48" s="53"/>
-      <c r="H48" s="54"/>
-      <c r="I48" s="44"/>
-      <c r="J48" s="55"/>
-      <c r="K48" s="30">
+      <c r="A48" s="39"/>
+      <c r="B48" s="42"/>
+      <c r="C48" s="42"/>
+      <c r="D48" s="42"/>
+      <c r="E48" s="42"/>
+      <c r="F48" s="42"/>
+      <c r="G48" s="42"/>
+      <c r="H48" s="45"/>
+      <c r="I48" s="52"/>
+      <c r="K48" s="4">
         <v>5</v>
       </c>
-      <c r="L48" s="30" t="s">
+      <c r="L48" s="4" t="s">
         <v>130</v>
       </c>
-      <c r="M48" s="30" t="s">
+      <c r="M48" s="4" t="s">
         <v>135</v>
       </c>
-      <c r="N48" s="30" t="s">
+      <c r="N48" s="4" t="s">
         <v>135</v>
       </c>
-      <c r="O48" s="30" t="s">
-        <v>46</v>
-      </c>
-      <c r="P48" s="30"/>
-      <c r="Q48" s="56"/>
-      <c r="R48" s="19"/>
+      <c r="O48" s="4" t="s">
+        <v>46</v>
+      </c>
+      <c r="R48" s="36"/>
     </row>
     <row r="49" spans="1:18" ht="31.5" x14ac:dyDescent="0.2">
-      <c r="A49" s="28"/>
-      <c r="B49" s="53"/>
-      <c r="C49" s="53"/>
-      <c r="D49" s="53"/>
-      <c r="E49" s="53"/>
-      <c r="F49" s="53"/>
-      <c r="G49" s="53"/>
-      <c r="H49" s="54"/>
-      <c r="I49" s="44"/>
-      <c r="J49" s="55"/>
-      <c r="K49" s="30">
+      <c r="A49" s="39"/>
+      <c r="B49" s="42"/>
+      <c r="C49" s="42"/>
+      <c r="D49" s="42"/>
+      <c r="E49" s="42"/>
+      <c r="F49" s="42"/>
+      <c r="G49" s="42"/>
+      <c r="H49" s="45"/>
+      <c r="I49" s="52"/>
+      <c r="K49" s="4">
         <v>6</v>
       </c>
-      <c r="L49" s="30" t="s">
+      <c r="L49" s="4" t="s">
         <v>51</v>
       </c>
-      <c r="M49" s="30" t="s">
+      <c r="M49" s="4" t="s">
         <v>138</v>
       </c>
-      <c r="N49" s="30" t="s">
+      <c r="N49" s="4" t="s">
         <v>109</v>
       </c>
-      <c r="O49" s="30" t="s">
+      <c r="O49" s="4" t="s">
         <v>89</v>
       </c>
-      <c r="P49" s="57" t="s">
+      <c r="P49" s="31" t="s">
         <v>154</v>
       </c>
-      <c r="Q49" s="56" t="s">
+      <c r="Q49" s="26" t="s">
         <v>149</v>
       </c>
-      <c r="R49" s="19"/>
+      <c r="R49" s="36"/>
     </row>
     <row r="50" spans="1:18" ht="24" x14ac:dyDescent="0.2">
-      <c r="A50" s="28"/>
-      <c r="B50" s="53"/>
-      <c r="C50" s="53"/>
-      <c r="D50" s="53"/>
-      <c r="E50" s="53"/>
-      <c r="F50" s="53"/>
-      <c r="G50" s="53"/>
-      <c r="H50" s="54"/>
-      <c r="I50" s="44"/>
-      <c r="J50" s="55"/>
-      <c r="K50" s="30">
+      <c r="A50" s="39"/>
+      <c r="B50" s="42"/>
+      <c r="C50" s="42"/>
+      <c r="D50" s="42"/>
+      <c r="E50" s="42"/>
+      <c r="F50" s="42"/>
+      <c r="G50" s="42"/>
+      <c r="H50" s="45"/>
+      <c r="I50" s="52"/>
+      <c r="K50" s="4">
         <v>7</v>
       </c>
-      <c r="L50" s="30" t="s">
+      <c r="L50" s="4" t="s">
         <v>132</v>
       </c>
-      <c r="M50" s="30" t="s">
+      <c r="M50" s="4" t="s">
         <v>136</v>
       </c>
-      <c r="N50" s="30" t="s">
+      <c r="N50" s="4" t="s">
         <v>136</v>
       </c>
-      <c r="O50" s="30" t="s">
-        <v>46</v>
-      </c>
-      <c r="P50" s="30"/>
-      <c r="Q50" s="56"/>
-      <c r="R50" s="19"/>
+      <c r="O50" s="4" t="s">
+        <v>46</v>
+      </c>
+      <c r="R50" s="36"/>
     </row>
     <row r="51" spans="1:18" ht="24" x14ac:dyDescent="0.2">
-      <c r="A51" s="28"/>
-      <c r="B51" s="53"/>
-      <c r="C51" s="53"/>
-      <c r="D51" s="53"/>
-      <c r="E51" s="53"/>
-      <c r="F51" s="53"/>
-      <c r="G51" s="53"/>
-      <c r="H51" s="54"/>
-      <c r="I51" s="44"/>
-      <c r="J51" s="55"/>
-      <c r="K51" s="30">
+      <c r="A51" s="39"/>
+      <c r="B51" s="42"/>
+      <c r="C51" s="42"/>
+      <c r="D51" s="42"/>
+      <c r="E51" s="42"/>
+      <c r="F51" s="42"/>
+      <c r="G51" s="42"/>
+      <c r="H51" s="45"/>
+      <c r="I51" s="52"/>
+      <c r="K51" s="4">
         <v>8</v>
       </c>
-      <c r="L51" s="30" t="s">
+      <c r="L51" s="4" t="s">
         <v>51</v>
       </c>
-      <c r="M51" s="30" t="s">
+      <c r="M51" s="4" t="s">
         <v>138</v>
       </c>
-      <c r="N51" s="30" t="s">
+      <c r="N51" s="4" t="s">
         <v>138</v>
       </c>
-      <c r="O51" s="30" t="s">
-        <v>46</v>
-      </c>
-      <c r="P51" s="30"/>
-      <c r="Q51" s="56"/>
-      <c r="R51" s="19"/>
+      <c r="O51" s="4" t="s">
+        <v>46</v>
+      </c>
+      <c r="R51" s="36"/>
     </row>
     <row r="52" spans="1:18" ht="24" x14ac:dyDescent="0.2">
-      <c r="A52" s="28"/>
-      <c r="B52" s="53"/>
-      <c r="C52" s="53"/>
-      <c r="D52" s="53"/>
-      <c r="E52" s="53"/>
-      <c r="F52" s="53"/>
-      <c r="G52" s="53"/>
-      <c r="H52" s="54"/>
-      <c r="I52" s="44"/>
-      <c r="J52" s="55"/>
-      <c r="K52" s="30">
+      <c r="A52" s="39"/>
+      <c r="B52" s="42"/>
+      <c r="C52" s="42"/>
+      <c r="D52" s="42"/>
+      <c r="E52" s="42"/>
+      <c r="F52" s="42"/>
+      <c r="G52" s="42"/>
+      <c r="H52" s="45"/>
+      <c r="I52" s="52"/>
+      <c r="K52" s="4">
         <v>9</v>
       </c>
-      <c r="L52" s="30" t="s">
+      <c r="L52" s="4" t="s">
         <v>131</v>
       </c>
-      <c r="M52" s="30" t="s">
+      <c r="M52" s="4" t="s">
         <v>137</v>
       </c>
-      <c r="N52" s="30" t="s">
+      <c r="N52" s="4" t="s">
         <v>137</v>
       </c>
-      <c r="O52" s="30" t="s">
-        <v>46</v>
-      </c>
-      <c r="P52" s="30"/>
-      <c r="Q52" s="56"/>
-      <c r="R52" s="19"/>
+      <c r="O52" s="4" t="s">
+        <v>46</v>
+      </c>
+      <c r="R52" s="36"/>
     </row>
     <row r="53" spans="1:18" ht="32.25" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A53" s="29"/>
-      <c r="B53" s="23"/>
-      <c r="C53" s="23"/>
-      <c r="D53" s="23"/>
-      <c r="E53" s="23"/>
-      <c r="F53" s="23"/>
-      <c r="G53" s="23"/>
-      <c r="H53" s="26"/>
-      <c r="I53" s="45"/>
-      <c r="J53" s="41"/>
+      <c r="A53" s="40"/>
+      <c r="B53" s="43"/>
+      <c r="C53" s="43"/>
+      <c r="D53" s="43"/>
+      <c r="E53" s="43"/>
+      <c r="F53" s="43"/>
+      <c r="G53" s="43"/>
+      <c r="H53" s="46"/>
+      <c r="I53" s="53"/>
+      <c r="J53" s="23"/>
       <c r="K53" s="14">
         <v>10</v>
       </c>
@@ -3676,26 +3590,60 @@
       <c r="O53" s="14" t="s">
         <v>89</v>
       </c>
-      <c r="P53" s="58" t="s">
+      <c r="P53" s="32" t="s">
         <v>154</v>
       </c>
-      <c r="Q53" s="49" t="s">
+      <c r="Q53" s="27" t="s">
         <v>149</v>
       </c>
-      <c r="R53" s="20"/>
+      <c r="R53" s="37"/>
     </row>
   </sheetData>
   <mergeCells count="70">
-    <mergeCell ref="R41:R43"/>
-    <mergeCell ref="A41:A43"/>
-    <mergeCell ref="C41:C43"/>
-    <mergeCell ref="D41:D43"/>
-    <mergeCell ref="E41:E43"/>
-    <mergeCell ref="F41:F43"/>
-    <mergeCell ref="G41:G43"/>
-    <mergeCell ref="B41:B43"/>
-    <mergeCell ref="H41:H43"/>
-    <mergeCell ref="I41:I43"/>
+    <mergeCell ref="A44:A53"/>
+    <mergeCell ref="C44:C53"/>
+    <mergeCell ref="D44:D53"/>
+    <mergeCell ref="E44:E53"/>
+    <mergeCell ref="R44:R53"/>
+    <mergeCell ref="F44:F53"/>
+    <mergeCell ref="G44:G53"/>
+    <mergeCell ref="B44:B53"/>
+    <mergeCell ref="H44:H53"/>
+    <mergeCell ref="I44:I53"/>
+    <mergeCell ref="R2:R8"/>
+    <mergeCell ref="I2:I8"/>
+    <mergeCell ref="G2:G8"/>
+    <mergeCell ref="B2:B8"/>
+    <mergeCell ref="H2:H8"/>
+    <mergeCell ref="A2:A8"/>
+    <mergeCell ref="C2:C8"/>
+    <mergeCell ref="D2:D8"/>
+    <mergeCell ref="E2:E8"/>
+    <mergeCell ref="A9:A16"/>
+    <mergeCell ref="C9:C16"/>
+    <mergeCell ref="D9:D16"/>
+    <mergeCell ref="E9:E16"/>
+    <mergeCell ref="G9:G16"/>
+    <mergeCell ref="B9:B16"/>
+    <mergeCell ref="H9:H16"/>
+    <mergeCell ref="I9:I16"/>
+    <mergeCell ref="F2:F8"/>
+    <mergeCell ref="A26:A34"/>
+    <mergeCell ref="C26:C34"/>
+    <mergeCell ref="D26:D34"/>
+    <mergeCell ref="E26:E34"/>
+    <mergeCell ref="R9:R16"/>
+    <mergeCell ref="A17:A25"/>
+    <mergeCell ref="C17:C25"/>
+    <mergeCell ref="D17:D25"/>
+    <mergeCell ref="E17:E25"/>
+    <mergeCell ref="F17:F25"/>
+    <mergeCell ref="G17:G25"/>
+    <mergeCell ref="B17:B25"/>
+    <mergeCell ref="H17:H25"/>
+    <mergeCell ref="I17:I25"/>
+    <mergeCell ref="R17:R25"/>
+    <mergeCell ref="F9:F16"/>
     <mergeCell ref="R26:R34"/>
     <mergeCell ref="A35:A40"/>
     <mergeCell ref="C35:C40"/>
@@ -3712,89 +3660,50 @@
     <mergeCell ref="B26:B34"/>
     <mergeCell ref="H26:H34"/>
     <mergeCell ref="I26:I34"/>
-    <mergeCell ref="A26:A34"/>
-    <mergeCell ref="C26:C34"/>
-    <mergeCell ref="D26:D34"/>
-    <mergeCell ref="E26:E34"/>
-    <mergeCell ref="R9:R16"/>
-    <mergeCell ref="A17:A25"/>
-    <mergeCell ref="C17:C25"/>
-    <mergeCell ref="D17:D25"/>
-    <mergeCell ref="E17:E25"/>
-    <mergeCell ref="F17:F25"/>
-    <mergeCell ref="G17:G25"/>
-    <mergeCell ref="B17:B25"/>
-    <mergeCell ref="H17:H25"/>
-    <mergeCell ref="I17:I25"/>
-    <mergeCell ref="R17:R25"/>
-    <mergeCell ref="F9:F16"/>
-    <mergeCell ref="G9:G16"/>
-    <mergeCell ref="B9:B16"/>
-    <mergeCell ref="H9:H16"/>
-    <mergeCell ref="I9:I16"/>
-    <mergeCell ref="F2:F8"/>
-    <mergeCell ref="A2:A8"/>
-    <mergeCell ref="C2:C8"/>
-    <mergeCell ref="D2:D8"/>
-    <mergeCell ref="E2:E8"/>
-    <mergeCell ref="A9:A16"/>
-    <mergeCell ref="C9:C16"/>
-    <mergeCell ref="D9:D16"/>
-    <mergeCell ref="E9:E16"/>
-    <mergeCell ref="R2:R8"/>
-    <mergeCell ref="I2:I8"/>
-    <mergeCell ref="G2:G8"/>
-    <mergeCell ref="B2:B8"/>
-    <mergeCell ref="H2:H8"/>
-    <mergeCell ref="A44:A53"/>
-    <mergeCell ref="C44:C53"/>
-    <mergeCell ref="D44:D53"/>
-    <mergeCell ref="E44:E53"/>
-    <mergeCell ref="R44:R53"/>
-    <mergeCell ref="F44:F53"/>
-    <mergeCell ref="G44:G53"/>
-    <mergeCell ref="B44:B53"/>
-    <mergeCell ref="H44:H53"/>
-    <mergeCell ref="I44:I53"/>
+    <mergeCell ref="R41:R43"/>
+    <mergeCell ref="A41:A43"/>
+    <mergeCell ref="C41:C43"/>
+    <mergeCell ref="D41:D43"/>
+    <mergeCell ref="E41:E43"/>
+    <mergeCell ref="F41:F43"/>
+    <mergeCell ref="G41:G43"/>
+    <mergeCell ref="B41:B43"/>
+    <mergeCell ref="H41:H43"/>
+    <mergeCell ref="I41:I43"/>
   </mergeCells>
   <conditionalFormatting sqref="B1:B1048576 I9">
-    <cfRule type="cellIs" dxfId="10" priority="10" operator="equal">
+    <cfRule type="cellIs" dxfId="19" priority="10" operator="equal">
       <formula>"NIE"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="9" priority="11" operator="equal">
+    <cfRule type="cellIs" dxfId="18" priority="11" operator="equal">
       <formula>"tak"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="O1:O1048576">
-    <cfRule type="cellIs" dxfId="8" priority="8" operator="equal">
+    <cfRule type="cellIs" dxfId="17" priority="8" operator="equal">
       <formula>"TAK"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="7" priority="9" operator="equal">
+    <cfRule type="cellIs" dxfId="16" priority="9" operator="equal">
       <formula>"NIE"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="Q1:Q1048576">
-    <cfRule type="cellIs" dxfId="6" priority="1" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="15" priority="1" stopIfTrue="1" operator="equal">
       <formula>"BŁĄD KRYTYCZNY"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="5" priority="2" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="14" priority="2" stopIfTrue="1" operator="equal">
       <formula>"BŁĄD ISTOTNY"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="4" priority="3" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="13" priority="3" stopIfTrue="1" operator="equal">
       <formula>"BŁĄD"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="3" priority="4" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="12" priority="4" stopIfTrue="1" operator="equal">
       <formula>"ISTOTNA USTERKA"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="2" priority="5" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="11" priority="5" stopIfTrue="1" operator="equal">
       <formula>"USTERKA"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="0" priority="6" stopIfTrue="1" operator="equal">
-      <formula>"USTERKA PODRZĘDNA"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="Q4">
-    <cfRule type="cellIs" dxfId="1" priority="7" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="10" priority="6" stopIfTrue="1" operator="equal">
       <formula>"USTERKA PODRZĘDNA"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -3818,4 +3727,1182 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId8"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{02FAEA6D-28C9-4A30-A6D3-1472532CD6D8}">
+  <dimension ref="A1:S33"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane xSplit="2" ySplit="1" topLeftCell="C17" activePane="bottomRight" state="frozen"/>
+      <selection pane="topRight" activeCell="C1" sqref="C1"/>
+      <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
+      <selection pane="bottomRight" activeCell="R20" sqref="R20:R33"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="8.28515625" style="4" customWidth="1"/>
+    <col min="2" max="2" width="5.42578125" style="4" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="12.5703125" style="4" customWidth="1"/>
+    <col min="4" max="4" width="29" style="4" customWidth="1"/>
+    <col min="5" max="5" width="19.85546875" style="4" customWidth="1"/>
+    <col min="6" max="6" width="6.5703125" style="4" customWidth="1"/>
+    <col min="7" max="7" width="10.28515625" style="4" customWidth="1"/>
+    <col min="8" max="8" width="9" style="4" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="6.42578125" style="4" customWidth="1"/>
+    <col min="10" max="10" width="1.7109375" style="22" customWidth="1"/>
+    <col min="11" max="11" width="5" style="4" customWidth="1"/>
+    <col min="12" max="12" width="21.42578125" style="4" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="23.7109375" style="4" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="25.140625" style="4" customWidth="1"/>
+    <col min="15" max="15" width="5.85546875" style="4" customWidth="1"/>
+    <col min="16" max="16" width="14.42578125" style="4" customWidth="1"/>
+    <col min="17" max="17" width="13.42578125" style="26" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="14.42578125" style="4" customWidth="1"/>
+    <col min="19" max="19" width="22.85546875" style="4" customWidth="1"/>
+    <col min="20" max="16384" width="9.140625" style="20"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:19" s="16" customFormat="1" ht="24.75" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="7" t="s">
+        <v>14</v>
+      </c>
+      <c r="B1" s="6" t="s">
+        <v>140</v>
+      </c>
+      <c r="C1" s="6" t="s">
+        <v>141</v>
+      </c>
+      <c r="D1" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="E1" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="F1" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="G1" s="6" t="s">
+        <v>17</v>
+      </c>
+      <c r="H1" s="6" t="s">
+        <v>34</v>
+      </c>
+      <c r="I1" s="6" t="s">
+        <v>24</v>
+      </c>
+      <c r="J1" s="17"/>
+      <c r="K1" s="6" t="s">
+        <v>29</v>
+      </c>
+      <c r="L1" s="6" t="s">
+        <v>18</v>
+      </c>
+      <c r="M1" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="N1" s="6" t="s">
+        <v>20</v>
+      </c>
+      <c r="O1" s="6" t="s">
+        <v>31</v>
+      </c>
+      <c r="P1" s="6" t="s">
+        <v>22</v>
+      </c>
+      <c r="Q1" s="24" t="s">
+        <v>25</v>
+      </c>
+      <c r="R1" s="18" t="s">
+        <v>23</v>
+      </c>
+      <c r="S1" s="19"/>
+    </row>
+    <row r="2" spans="1:19" ht="24" x14ac:dyDescent="0.2">
+      <c r="A2" s="54" t="s">
+        <v>156</v>
+      </c>
+      <c r="B2" s="41" t="s">
+        <v>89</v>
+      </c>
+      <c r="C2" s="41" t="s">
+        <v>168</v>
+      </c>
+      <c r="D2" s="41" t="s">
+        <v>189</v>
+      </c>
+      <c r="E2" s="41" t="s">
+        <v>157</v>
+      </c>
+      <c r="F2" s="41">
+        <v>1</v>
+      </c>
+      <c r="G2" s="41" t="s">
+        <v>45</v>
+      </c>
+      <c r="H2" s="44" t="s">
+        <v>190</v>
+      </c>
+      <c r="I2" s="47"/>
+      <c r="J2" s="21"/>
+      <c r="K2" s="13">
+        <v>1</v>
+      </c>
+      <c r="L2" s="13" t="s">
+        <v>178</v>
+      </c>
+      <c r="M2" s="13" t="s">
+        <v>158</v>
+      </c>
+      <c r="N2" s="13" t="s">
+        <v>158</v>
+      </c>
+      <c r="O2" s="13" t="s">
+        <v>46</v>
+      </c>
+      <c r="P2" s="13"/>
+      <c r="Q2" s="25"/>
+      <c r="R2" s="35"/>
+    </row>
+    <row r="3" spans="1:19" ht="24" x14ac:dyDescent="0.2">
+      <c r="A3" s="39"/>
+      <c r="B3" s="42"/>
+      <c r="C3" s="42"/>
+      <c r="D3" s="42"/>
+      <c r="E3" s="42"/>
+      <c r="F3" s="42"/>
+      <c r="G3" s="42"/>
+      <c r="H3" s="45"/>
+      <c r="I3" s="48"/>
+      <c r="K3" s="4">
+        <v>2</v>
+      </c>
+      <c r="L3" s="4" t="s">
+        <v>165</v>
+      </c>
+      <c r="M3" s="4" t="s">
+        <v>174</v>
+      </c>
+      <c r="N3" s="4" t="s">
+        <v>174</v>
+      </c>
+      <c r="O3" s="4" t="s">
+        <v>46</v>
+      </c>
+      <c r="R3" s="36"/>
+    </row>
+    <row r="4" spans="1:19" ht="24" x14ac:dyDescent="0.2">
+      <c r="A4" s="39"/>
+      <c r="B4" s="42"/>
+      <c r="C4" s="42"/>
+      <c r="D4" s="42"/>
+      <c r="E4" s="42"/>
+      <c r="F4" s="42"/>
+      <c r="G4" s="42"/>
+      <c r="H4" s="45"/>
+      <c r="I4" s="48"/>
+      <c r="K4" s="4">
+        <v>3</v>
+      </c>
+      <c r="L4" s="4" t="s">
+        <v>177</v>
+      </c>
+      <c r="M4" s="4" t="s">
+        <v>159</v>
+      </c>
+      <c r="N4" s="4" t="s">
+        <v>159</v>
+      </c>
+      <c r="O4" s="4" t="s">
+        <v>46</v>
+      </c>
+      <c r="R4" s="36"/>
+    </row>
+    <row r="5" spans="1:19" ht="24" x14ac:dyDescent="0.2">
+      <c r="A5" s="39"/>
+      <c r="B5" s="42"/>
+      <c r="C5" s="42"/>
+      <c r="D5" s="42"/>
+      <c r="E5" s="42"/>
+      <c r="F5" s="42"/>
+      <c r="G5" s="42"/>
+      <c r="H5" s="45"/>
+      <c r="I5" s="48"/>
+      <c r="K5" s="4">
+        <v>4</v>
+      </c>
+      <c r="L5" s="4" t="s">
+        <v>165</v>
+      </c>
+      <c r="M5" s="4" t="s">
+        <v>174</v>
+      </c>
+      <c r="N5" s="4" t="s">
+        <v>174</v>
+      </c>
+      <c r="O5" s="4" t="s">
+        <v>46</v>
+      </c>
+      <c r="R5" s="36"/>
+    </row>
+    <row r="6" spans="1:19" ht="48" x14ac:dyDescent="0.2">
+      <c r="A6" s="39"/>
+      <c r="B6" s="42"/>
+      <c r="C6" s="42"/>
+      <c r="D6" s="42"/>
+      <c r="E6" s="42"/>
+      <c r="F6" s="42"/>
+      <c r="G6" s="42"/>
+      <c r="H6" s="45"/>
+      <c r="I6" s="48"/>
+      <c r="K6" s="4">
+        <v>5</v>
+      </c>
+      <c r="L6" s="4" t="s">
+        <v>176</v>
+      </c>
+      <c r="M6" s="4" t="s">
+        <v>160</v>
+      </c>
+      <c r="N6" s="4" t="s">
+        <v>179</v>
+      </c>
+      <c r="O6" s="4" t="s">
+        <v>89</v>
+      </c>
+      <c r="P6" s="4" t="s">
+        <v>180</v>
+      </c>
+      <c r="Q6" s="26" t="s">
+        <v>181</v>
+      </c>
+      <c r="R6" s="36"/>
+    </row>
+    <row r="7" spans="1:19" ht="24" x14ac:dyDescent="0.2">
+      <c r="A7" s="39"/>
+      <c r="B7" s="42"/>
+      <c r="C7" s="42"/>
+      <c r="D7" s="42"/>
+      <c r="E7" s="42"/>
+      <c r="F7" s="42"/>
+      <c r="G7" s="42"/>
+      <c r="H7" s="45"/>
+      <c r="I7" s="48"/>
+      <c r="K7" s="4">
+        <v>6</v>
+      </c>
+      <c r="L7" s="4" t="s">
+        <v>165</v>
+      </c>
+      <c r="M7" s="4" t="s">
+        <v>174</v>
+      </c>
+      <c r="N7" s="4" t="s">
+        <v>174</v>
+      </c>
+      <c r="O7" s="4" t="s">
+        <v>46</v>
+      </c>
+      <c r="R7" s="36"/>
+    </row>
+    <row r="8" spans="1:19" ht="24" x14ac:dyDescent="0.2">
+      <c r="A8" s="39"/>
+      <c r="B8" s="42"/>
+      <c r="C8" s="42"/>
+      <c r="D8" s="42"/>
+      <c r="E8" s="42"/>
+      <c r="F8" s="42"/>
+      <c r="G8" s="42"/>
+      <c r="H8" s="45"/>
+      <c r="I8" s="48"/>
+      <c r="K8" s="4">
+        <v>7</v>
+      </c>
+      <c r="L8" s="4" t="s">
+        <v>175</v>
+      </c>
+      <c r="M8" s="4" t="s">
+        <v>169</v>
+      </c>
+      <c r="N8" s="4" t="s">
+        <v>169</v>
+      </c>
+      <c r="O8" s="4" t="s">
+        <v>89</v>
+      </c>
+      <c r="P8" s="4" t="s">
+        <v>182</v>
+      </c>
+      <c r="Q8" s="26" t="s">
+        <v>184</v>
+      </c>
+      <c r="R8" s="36"/>
+    </row>
+    <row r="9" spans="1:19" ht="108" x14ac:dyDescent="0.2">
+      <c r="A9" s="39"/>
+      <c r="B9" s="42"/>
+      <c r="C9" s="42"/>
+      <c r="D9" s="42"/>
+      <c r="E9" s="42"/>
+      <c r="F9" s="42"/>
+      <c r="G9" s="42"/>
+      <c r="H9" s="45"/>
+      <c r="I9" s="48"/>
+      <c r="K9" s="4">
+        <v>8</v>
+      </c>
+      <c r="L9" s="4" t="s">
+        <v>165</v>
+      </c>
+      <c r="M9" s="4" t="s">
+        <v>174</v>
+      </c>
+      <c r="N9" s="4" t="s">
+        <v>174</v>
+      </c>
+      <c r="O9" s="4" t="s">
+        <v>89</v>
+      </c>
+      <c r="P9" s="4" t="s">
+        <v>183</v>
+      </c>
+      <c r="Q9" s="26" t="s">
+        <v>151</v>
+      </c>
+      <c r="R9" s="36"/>
+    </row>
+    <row r="10" spans="1:19" ht="108" x14ac:dyDescent="0.2">
+      <c r="A10" s="39"/>
+      <c r="B10" s="42"/>
+      <c r="C10" s="42"/>
+      <c r="D10" s="42"/>
+      <c r="E10" s="42"/>
+      <c r="F10" s="42"/>
+      <c r="G10" s="42"/>
+      <c r="H10" s="45"/>
+      <c r="I10" s="48"/>
+      <c r="K10" s="4">
+        <v>9</v>
+      </c>
+      <c r="L10" s="4" t="s">
+        <v>170</v>
+      </c>
+      <c r="M10" s="4" t="s">
+        <v>161</v>
+      </c>
+      <c r="N10" s="4" t="s">
+        <v>161</v>
+      </c>
+      <c r="O10" s="4" t="s">
+        <v>89</v>
+      </c>
+      <c r="P10" s="4" t="s">
+        <v>187</v>
+      </c>
+      <c r="Q10" s="26" t="s">
+        <v>151</v>
+      </c>
+      <c r="R10" s="36"/>
+    </row>
+    <row r="11" spans="1:19" ht="108" x14ac:dyDescent="0.2">
+      <c r="A11" s="39"/>
+      <c r="B11" s="42"/>
+      <c r="C11" s="42"/>
+      <c r="D11" s="42"/>
+      <c r="E11" s="42"/>
+      <c r="F11" s="42"/>
+      <c r="G11" s="42"/>
+      <c r="H11" s="45"/>
+      <c r="I11" s="48"/>
+      <c r="K11" s="4">
+        <v>10</v>
+      </c>
+      <c r="L11" s="4" t="s">
+        <v>165</v>
+      </c>
+      <c r="M11" s="4" t="s">
+        <v>174</v>
+      </c>
+      <c r="N11" s="4" t="s">
+        <v>174</v>
+      </c>
+      <c r="O11" s="4" t="s">
+        <v>89</v>
+      </c>
+      <c r="P11" s="4" t="s">
+        <v>185</v>
+      </c>
+      <c r="Q11" s="26" t="s">
+        <v>151</v>
+      </c>
+      <c r="R11" s="36"/>
+    </row>
+    <row r="12" spans="1:19" ht="24" x14ac:dyDescent="0.2">
+      <c r="A12" s="39"/>
+      <c r="B12" s="42"/>
+      <c r="C12" s="42"/>
+      <c r="D12" s="42"/>
+      <c r="E12" s="42"/>
+      <c r="F12" s="42"/>
+      <c r="G12" s="42"/>
+      <c r="H12" s="45"/>
+      <c r="I12" s="48"/>
+      <c r="K12" s="4">
+        <v>11</v>
+      </c>
+      <c r="L12" s="4" t="s">
+        <v>163</v>
+      </c>
+      <c r="M12" s="4" t="s">
+        <v>162</v>
+      </c>
+      <c r="N12" s="4" t="s">
+        <v>162</v>
+      </c>
+      <c r="O12" s="4" t="s">
+        <v>46</v>
+      </c>
+      <c r="R12" s="36"/>
+    </row>
+    <row r="13" spans="1:19" ht="24" x14ac:dyDescent="0.2">
+      <c r="A13" s="39"/>
+      <c r="B13" s="42"/>
+      <c r="C13" s="42"/>
+      <c r="D13" s="42"/>
+      <c r="E13" s="42"/>
+      <c r="F13" s="42"/>
+      <c r="G13" s="42"/>
+      <c r="H13" s="45"/>
+      <c r="I13" s="48"/>
+      <c r="K13" s="4">
+        <v>12</v>
+      </c>
+      <c r="L13" s="4" t="s">
+        <v>165</v>
+      </c>
+      <c r="M13" s="4" t="s">
+        <v>174</v>
+      </c>
+      <c r="N13" s="4" t="s">
+        <v>174</v>
+      </c>
+      <c r="O13" s="4" t="s">
+        <v>46</v>
+      </c>
+      <c r="R13" s="36"/>
+    </row>
+    <row r="14" spans="1:19" ht="24" x14ac:dyDescent="0.2">
+      <c r="A14" s="39"/>
+      <c r="B14" s="42"/>
+      <c r="C14" s="42"/>
+      <c r="D14" s="42"/>
+      <c r="E14" s="42"/>
+      <c r="F14" s="42"/>
+      <c r="G14" s="42"/>
+      <c r="H14" s="45"/>
+      <c r="I14" s="48"/>
+      <c r="K14" s="4">
+        <v>13</v>
+      </c>
+      <c r="L14" s="4" t="s">
+        <v>171</v>
+      </c>
+      <c r="M14" s="4" t="s">
+        <v>164</v>
+      </c>
+      <c r="N14" s="4" t="s">
+        <v>164</v>
+      </c>
+      <c r="O14" s="4" t="s">
+        <v>46</v>
+      </c>
+      <c r="R14" s="36"/>
+    </row>
+    <row r="15" spans="1:19" ht="24" x14ac:dyDescent="0.2">
+      <c r="A15" s="39"/>
+      <c r="B15" s="42"/>
+      <c r="C15" s="42"/>
+      <c r="D15" s="42"/>
+      <c r="E15" s="42"/>
+      <c r="F15" s="42"/>
+      <c r="G15" s="42"/>
+      <c r="H15" s="45"/>
+      <c r="I15" s="48"/>
+      <c r="K15" s="4">
+        <v>14</v>
+      </c>
+      <c r="L15" s="4" t="s">
+        <v>165</v>
+      </c>
+      <c r="M15" s="4" t="s">
+        <v>174</v>
+      </c>
+      <c r="N15" s="4" t="s">
+        <v>174</v>
+      </c>
+      <c r="O15" s="4" t="s">
+        <v>46</v>
+      </c>
+      <c r="R15" s="36"/>
+    </row>
+    <row r="16" spans="1:19" ht="24" x14ac:dyDescent="0.2">
+      <c r="A16" s="39"/>
+      <c r="B16" s="42"/>
+      <c r="C16" s="42"/>
+      <c r="D16" s="42"/>
+      <c r="E16" s="42"/>
+      <c r="F16" s="42"/>
+      <c r="G16" s="42"/>
+      <c r="H16" s="45"/>
+      <c r="I16" s="48"/>
+      <c r="K16" s="4">
+        <v>15</v>
+      </c>
+      <c r="L16" s="4" t="s">
+        <v>172</v>
+      </c>
+      <c r="M16" s="4" t="s">
+        <v>166</v>
+      </c>
+      <c r="N16" s="4" t="s">
+        <v>166</v>
+      </c>
+      <c r="O16" s="4" t="s">
+        <v>46</v>
+      </c>
+      <c r="R16" s="36"/>
+    </row>
+    <row r="17" spans="1:18" ht="24" x14ac:dyDescent="0.2">
+      <c r="A17" s="39"/>
+      <c r="B17" s="42"/>
+      <c r="C17" s="42"/>
+      <c r="D17" s="42"/>
+      <c r="E17" s="42"/>
+      <c r="F17" s="42"/>
+      <c r="G17" s="42"/>
+      <c r="H17" s="45"/>
+      <c r="I17" s="48"/>
+      <c r="K17" s="4">
+        <v>16</v>
+      </c>
+      <c r="L17" s="4" t="s">
+        <v>165</v>
+      </c>
+      <c r="M17" s="4" t="s">
+        <v>174</v>
+      </c>
+      <c r="N17" s="4" t="s">
+        <v>174</v>
+      </c>
+      <c r="O17" s="4" t="s">
+        <v>46</v>
+      </c>
+      <c r="R17" s="36"/>
+    </row>
+    <row r="18" spans="1:18" ht="24" x14ac:dyDescent="0.2">
+      <c r="A18" s="39"/>
+      <c r="B18" s="42"/>
+      <c r="C18" s="42"/>
+      <c r="D18" s="42"/>
+      <c r="E18" s="42"/>
+      <c r="F18" s="42"/>
+      <c r="G18" s="42"/>
+      <c r="H18" s="45"/>
+      <c r="I18" s="48"/>
+      <c r="K18" s="4">
+        <v>17</v>
+      </c>
+      <c r="L18" s="4" t="s">
+        <v>173</v>
+      </c>
+      <c r="M18" s="4" t="s">
+        <v>167</v>
+      </c>
+      <c r="N18" s="4" t="s">
+        <v>167</v>
+      </c>
+      <c r="O18" s="4" t="s">
+        <v>89</v>
+      </c>
+      <c r="P18" s="4" t="s">
+        <v>186</v>
+      </c>
+      <c r="Q18" s="26" t="s">
+        <v>184</v>
+      </c>
+      <c r="R18" s="36"/>
+    </row>
+    <row r="19" spans="1:18" ht="84.75" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A19" s="40"/>
+      <c r="B19" s="43"/>
+      <c r="C19" s="43"/>
+      <c r="D19" s="43"/>
+      <c r="E19" s="43"/>
+      <c r="F19" s="43"/>
+      <c r="G19" s="43"/>
+      <c r="H19" s="46"/>
+      <c r="I19" s="49"/>
+      <c r="J19" s="23"/>
+      <c r="K19" s="14">
+        <v>18</v>
+      </c>
+      <c r="L19" s="14" t="s">
+        <v>165</v>
+      </c>
+      <c r="M19" s="14" t="s">
+        <v>174</v>
+      </c>
+      <c r="N19" s="14" t="s">
+        <v>174</v>
+      </c>
+      <c r="O19" s="14" t="s">
+        <v>89</v>
+      </c>
+      <c r="P19" s="14" t="s">
+        <v>188</v>
+      </c>
+      <c r="Q19" s="27" t="s">
+        <v>184</v>
+      </c>
+      <c r="R19" s="37"/>
+    </row>
+    <row r="20" spans="1:18" ht="24" x14ac:dyDescent="0.2">
+      <c r="A20" s="38" t="s">
+        <v>156</v>
+      </c>
+      <c r="B20" s="41"/>
+      <c r="C20" s="41" t="s">
+        <v>168</v>
+      </c>
+      <c r="D20" s="41" t="s">
+        <v>189</v>
+      </c>
+      <c r="E20" s="41" t="s">
+        <v>157</v>
+      </c>
+      <c r="F20" s="41">
+        <v>2</v>
+      </c>
+      <c r="G20" s="41" t="s">
+        <v>45</v>
+      </c>
+      <c r="H20" s="44"/>
+      <c r="I20" s="47"/>
+      <c r="J20" s="21"/>
+      <c r="K20" s="13">
+        <v>1</v>
+      </c>
+      <c r="L20" s="13" t="s">
+        <v>175</v>
+      </c>
+      <c r="M20" s="13" t="s">
+        <v>169</v>
+      </c>
+      <c r="N20" s="13" t="s">
+        <v>169</v>
+      </c>
+      <c r="O20" s="13" t="s">
+        <v>46</v>
+      </c>
+      <c r="P20" s="13"/>
+      <c r="Q20" s="25"/>
+      <c r="R20" s="35"/>
+    </row>
+    <row r="21" spans="1:18" ht="36" x14ac:dyDescent="0.2">
+      <c r="A21" s="39"/>
+      <c r="B21" s="55"/>
+      <c r="C21" s="55"/>
+      <c r="D21" s="55"/>
+      <c r="E21" s="55"/>
+      <c r="F21" s="55"/>
+      <c r="G21" s="55"/>
+      <c r="H21" s="56"/>
+      <c r="I21" s="48"/>
+      <c r="J21" s="57"/>
+      <c r="K21" s="58">
+        <v>2</v>
+      </c>
+      <c r="L21" s="58" t="s">
+        <v>193</v>
+      </c>
+      <c r="M21" s="58" t="s">
+        <v>191</v>
+      </c>
+      <c r="N21" s="58" t="s">
+        <v>199</v>
+      </c>
+      <c r="O21" s="58" t="s">
+        <v>89</v>
+      </c>
+      <c r="P21" s="58" t="s">
+        <v>206</v>
+      </c>
+      <c r="Q21" s="59" t="s">
+        <v>184</v>
+      </c>
+      <c r="R21" s="36"/>
+    </row>
+    <row r="22" spans="1:18" ht="24" x14ac:dyDescent="0.2">
+      <c r="A22" s="39"/>
+      <c r="B22" s="55"/>
+      <c r="C22" s="55"/>
+      <c r="D22" s="55"/>
+      <c r="E22" s="55"/>
+      <c r="F22" s="55"/>
+      <c r="G22" s="55"/>
+      <c r="H22" s="56"/>
+      <c r="I22" s="48"/>
+      <c r="J22" s="57"/>
+      <c r="K22" s="58">
+        <v>3</v>
+      </c>
+      <c r="L22" s="58" t="s">
+        <v>165</v>
+      </c>
+      <c r="M22" s="58" t="s">
+        <v>192</v>
+      </c>
+      <c r="N22" s="58" t="s">
+        <v>200</v>
+      </c>
+      <c r="O22" s="58" t="s">
+        <v>89</v>
+      </c>
+      <c r="P22" s="58" t="s">
+        <v>207</v>
+      </c>
+      <c r="Q22" s="59" t="s">
+        <v>150</v>
+      </c>
+      <c r="R22" s="36"/>
+    </row>
+    <row r="23" spans="1:18" ht="36" x14ac:dyDescent="0.2">
+      <c r="A23" s="39"/>
+      <c r="B23" s="55"/>
+      <c r="C23" s="55"/>
+      <c r="D23" s="55"/>
+      <c r="E23" s="55"/>
+      <c r="F23" s="55"/>
+      <c r="G23" s="55"/>
+      <c r="H23" s="56"/>
+      <c r="I23" s="48"/>
+      <c r="J23" s="57"/>
+      <c r="K23" s="58">
+        <v>4</v>
+      </c>
+      <c r="L23" s="58" t="s">
+        <v>165</v>
+      </c>
+      <c r="M23" s="58" t="s">
+        <v>194</v>
+      </c>
+      <c r="N23" s="58" t="s">
+        <v>194</v>
+      </c>
+      <c r="O23" s="58" t="s">
+        <v>46</v>
+      </c>
+      <c r="P23" s="58"/>
+      <c r="Q23" s="59"/>
+      <c r="R23" s="36"/>
+    </row>
+    <row r="24" spans="1:18" ht="36" x14ac:dyDescent="0.2">
+      <c r="A24" s="39"/>
+      <c r="B24" s="55"/>
+      <c r="C24" s="55"/>
+      <c r="D24" s="55"/>
+      <c r="E24" s="55"/>
+      <c r="F24" s="55"/>
+      <c r="G24" s="55"/>
+      <c r="H24" s="56"/>
+      <c r="I24" s="48"/>
+      <c r="J24" s="57"/>
+      <c r="K24" s="58">
+        <v>5</v>
+      </c>
+      <c r="L24" s="58" t="s">
+        <v>198</v>
+      </c>
+      <c r="M24" s="58" t="s">
+        <v>195</v>
+      </c>
+      <c r="N24" s="58" t="s">
+        <v>201</v>
+      </c>
+      <c r="O24" s="58" t="s">
+        <v>89</v>
+      </c>
+      <c r="P24" s="58" t="s">
+        <v>207</v>
+      </c>
+      <c r="Q24" s="59" t="s">
+        <v>150</v>
+      </c>
+      <c r="R24" s="36"/>
+    </row>
+    <row r="25" spans="1:18" ht="36" x14ac:dyDescent="0.2">
+      <c r="A25" s="39"/>
+      <c r="B25" s="55"/>
+      <c r="C25" s="55"/>
+      <c r="D25" s="55"/>
+      <c r="E25" s="55"/>
+      <c r="F25" s="55"/>
+      <c r="G25" s="55"/>
+      <c r="H25" s="56"/>
+      <c r="I25" s="48"/>
+      <c r="J25" s="57"/>
+      <c r="K25" s="58">
+        <v>6</v>
+      </c>
+      <c r="L25" s="58" t="s">
+        <v>193</v>
+      </c>
+      <c r="M25" s="58" t="s">
+        <v>191</v>
+      </c>
+      <c r="N25" s="58" t="s">
+        <v>199</v>
+      </c>
+      <c r="O25" s="58" t="s">
+        <v>89</v>
+      </c>
+      <c r="P25" s="58" t="s">
+        <v>206</v>
+      </c>
+      <c r="Q25" s="59" t="s">
+        <v>184</v>
+      </c>
+      <c r="R25" s="36"/>
+    </row>
+    <row r="26" spans="1:18" ht="24" x14ac:dyDescent="0.2">
+      <c r="A26" s="39"/>
+      <c r="B26" s="55"/>
+      <c r="C26" s="55"/>
+      <c r="D26" s="55"/>
+      <c r="E26" s="55"/>
+      <c r="F26" s="55"/>
+      <c r="G26" s="55"/>
+      <c r="H26" s="56"/>
+      <c r="I26" s="48"/>
+      <c r="J26" s="57"/>
+      <c r="K26" s="58">
+        <v>7</v>
+      </c>
+      <c r="L26" s="58" t="s">
+        <v>165</v>
+      </c>
+      <c r="M26" s="58" t="s">
+        <v>192</v>
+      </c>
+      <c r="N26" s="58" t="s">
+        <v>202</v>
+      </c>
+      <c r="O26" s="58" t="s">
+        <v>89</v>
+      </c>
+      <c r="P26" s="58" t="s">
+        <v>207</v>
+      </c>
+      <c r="Q26" s="59" t="s">
+        <v>150</v>
+      </c>
+      <c r="R26" s="36"/>
+    </row>
+    <row r="27" spans="1:18" ht="36" x14ac:dyDescent="0.2">
+      <c r="A27" s="39"/>
+      <c r="B27" s="55"/>
+      <c r="C27" s="55"/>
+      <c r="D27" s="55"/>
+      <c r="E27" s="55"/>
+      <c r="F27" s="55"/>
+      <c r="G27" s="55"/>
+      <c r="H27" s="56"/>
+      <c r="I27" s="48"/>
+      <c r="J27" s="57"/>
+      <c r="K27" s="58">
+        <v>8</v>
+      </c>
+      <c r="L27" s="58" t="s">
+        <v>165</v>
+      </c>
+      <c r="M27" s="58" t="s">
+        <v>194</v>
+      </c>
+      <c r="N27" s="58" t="s">
+        <v>202</v>
+      </c>
+      <c r="O27" s="58" t="s">
+        <v>89</v>
+      </c>
+      <c r="P27" s="58" t="s">
+        <v>207</v>
+      </c>
+      <c r="Q27" s="59" t="s">
+        <v>150</v>
+      </c>
+      <c r="R27" s="36"/>
+    </row>
+    <row r="28" spans="1:18" ht="24" x14ac:dyDescent="0.2">
+      <c r="A28" s="39"/>
+      <c r="B28" s="55"/>
+      <c r="C28" s="55"/>
+      <c r="D28" s="55"/>
+      <c r="E28" s="55"/>
+      <c r="F28" s="55"/>
+      <c r="G28" s="55"/>
+      <c r="H28" s="56"/>
+      <c r="I28" s="48"/>
+      <c r="J28" s="57"/>
+      <c r="K28" s="58">
+        <v>9</v>
+      </c>
+      <c r="L28" s="58" t="s">
+        <v>196</v>
+      </c>
+      <c r="M28" s="58" t="s">
+        <v>197</v>
+      </c>
+      <c r="N28" s="58" t="s">
+        <v>197</v>
+      </c>
+      <c r="O28" s="58" t="s">
+        <v>46</v>
+      </c>
+      <c r="P28" s="58"/>
+      <c r="Q28" s="59"/>
+      <c r="R28" s="36"/>
+    </row>
+    <row r="29" spans="1:18" ht="36" x14ac:dyDescent="0.2">
+      <c r="A29" s="39"/>
+      <c r="B29" s="55"/>
+      <c r="C29" s="55"/>
+      <c r="D29" s="55"/>
+      <c r="E29" s="55"/>
+      <c r="F29" s="55"/>
+      <c r="G29" s="55"/>
+      <c r="H29" s="56"/>
+      <c r="I29" s="48"/>
+      <c r="J29" s="57"/>
+      <c r="K29" s="58">
+        <v>10</v>
+      </c>
+      <c r="L29" s="58" t="s">
+        <v>173</v>
+      </c>
+      <c r="M29" s="58" t="s">
+        <v>203</v>
+      </c>
+      <c r="N29" s="58" t="s">
+        <v>204</v>
+      </c>
+      <c r="O29" s="58" t="s">
+        <v>89</v>
+      </c>
+      <c r="P29" s="58" t="s">
+        <v>207</v>
+      </c>
+      <c r="Q29" s="59" t="s">
+        <v>150</v>
+      </c>
+      <c r="R29" s="36"/>
+    </row>
+    <row r="30" spans="1:18" ht="36" x14ac:dyDescent="0.2">
+      <c r="A30" s="39"/>
+      <c r="B30" s="55"/>
+      <c r="C30" s="55"/>
+      <c r="D30" s="55"/>
+      <c r="E30" s="55"/>
+      <c r="F30" s="55"/>
+      <c r="G30" s="55"/>
+      <c r="H30" s="56"/>
+      <c r="I30" s="48"/>
+      <c r="J30" s="57"/>
+      <c r="K30" s="58">
+        <v>11</v>
+      </c>
+      <c r="L30" s="58" t="s">
+        <v>193</v>
+      </c>
+      <c r="M30" s="58" t="s">
+        <v>191</v>
+      </c>
+      <c r="N30" s="58" t="s">
+        <v>199</v>
+      </c>
+      <c r="O30" s="58" t="s">
+        <v>89</v>
+      </c>
+      <c r="P30" s="58" t="s">
+        <v>206</v>
+      </c>
+      <c r="Q30" s="59" t="s">
+        <v>184</v>
+      </c>
+      <c r="R30" s="36"/>
+    </row>
+    <row r="31" spans="1:18" ht="36" x14ac:dyDescent="0.2">
+      <c r="A31" s="39"/>
+      <c r="B31" s="55"/>
+      <c r="C31" s="55"/>
+      <c r="D31" s="55"/>
+      <c r="E31" s="55"/>
+      <c r="F31" s="55"/>
+      <c r="G31" s="55"/>
+      <c r="H31" s="56"/>
+      <c r="I31" s="48"/>
+      <c r="J31" s="57"/>
+      <c r="K31" s="58">
+        <v>12</v>
+      </c>
+      <c r="L31" s="58" t="s">
+        <v>165</v>
+      </c>
+      <c r="M31" s="58" t="s">
+        <v>192</v>
+      </c>
+      <c r="N31" s="58" t="s">
+        <v>204</v>
+      </c>
+      <c r="O31" s="58" t="s">
+        <v>89</v>
+      </c>
+      <c r="P31" s="58" t="s">
+        <v>208</v>
+      </c>
+      <c r="Q31" s="59" t="s">
+        <v>150</v>
+      </c>
+      <c r="R31" s="36"/>
+    </row>
+    <row r="32" spans="1:18" ht="36" x14ac:dyDescent="0.2">
+      <c r="A32" s="39"/>
+      <c r="B32" s="55"/>
+      <c r="C32" s="55"/>
+      <c r="D32" s="55"/>
+      <c r="E32" s="55"/>
+      <c r="F32" s="55"/>
+      <c r="G32" s="55"/>
+      <c r="H32" s="56"/>
+      <c r="I32" s="48"/>
+      <c r="J32" s="57"/>
+      <c r="K32" s="58"/>
+      <c r="L32" s="58" t="s">
+        <v>165</v>
+      </c>
+      <c r="M32" s="58" t="s">
+        <v>194</v>
+      </c>
+      <c r="N32" s="58" t="s">
+        <v>205</v>
+      </c>
+      <c r="O32" s="58" t="s">
+        <v>89</v>
+      </c>
+      <c r="P32" s="58"/>
+      <c r="Q32" s="59" t="s">
+        <v>181</v>
+      </c>
+      <c r="R32" s="36"/>
+    </row>
+    <row r="33" spans="1:18" ht="24.75" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A33" s="40"/>
+      <c r="B33" s="43"/>
+      <c r="C33" s="43"/>
+      <c r="D33" s="43"/>
+      <c r="E33" s="43"/>
+      <c r="F33" s="43"/>
+      <c r="G33" s="43"/>
+      <c r="H33" s="46"/>
+      <c r="I33" s="49"/>
+      <c r="J33" s="23"/>
+      <c r="K33" s="14">
+        <v>13</v>
+      </c>
+      <c r="L33" s="14" t="s">
+        <v>196</v>
+      </c>
+      <c r="M33" s="14" t="s">
+        <v>197</v>
+      </c>
+      <c r="N33" s="14" t="s">
+        <v>197</v>
+      </c>
+      <c r="O33" s="14" t="s">
+        <v>46</v>
+      </c>
+      <c r="P33" s="14"/>
+      <c r="Q33" s="27"/>
+      <c r="R33" s="37"/>
+    </row>
+  </sheetData>
+  <mergeCells count="20">
+    <mergeCell ref="F20:F33"/>
+    <mergeCell ref="G20:G33"/>
+    <mergeCell ref="H20:H33"/>
+    <mergeCell ref="I20:I33"/>
+    <mergeCell ref="R20:R33"/>
+    <mergeCell ref="A20:A33"/>
+    <mergeCell ref="B20:B33"/>
+    <mergeCell ref="C20:C33"/>
+    <mergeCell ref="D20:D33"/>
+    <mergeCell ref="E20:E33"/>
+    <mergeCell ref="G2:G19"/>
+    <mergeCell ref="H2:H19"/>
+    <mergeCell ref="I2:I19"/>
+    <mergeCell ref="R2:R19"/>
+    <mergeCell ref="A2:A19"/>
+    <mergeCell ref="B2:B19"/>
+    <mergeCell ref="C2:C19"/>
+    <mergeCell ref="D2:D19"/>
+    <mergeCell ref="E2:E19"/>
+    <mergeCell ref="F2:F19"/>
+  </mergeCells>
+  <conditionalFormatting sqref="B1:B1048576">
+    <cfRule type="cellIs" dxfId="9" priority="9" operator="equal">
+      <formula>"NIE"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="8" priority="10" operator="equal">
+      <formula>"tak"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="O1:O1048576">
+    <cfRule type="cellIs" dxfId="7" priority="7" operator="equal">
+      <formula>"TAK"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="6" priority="8" operator="equal">
+      <formula>"NIE"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="Q1:Q1048576">
+    <cfRule type="cellIs" dxfId="5" priority="1" stopIfTrue="1" operator="equal">
+      <formula>"BŁĄD KRYTYCZNY"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="4" priority="2" stopIfTrue="1" operator="equal">
+      <formula>"BŁĄD ISTOTNY"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="3" priority="3" stopIfTrue="1" operator="equal">
+      <formula>"BŁĄD"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="2" priority="4" stopIfTrue="1" operator="equal">
+      <formula>"ISTOTNA USTERKA"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="1" priority="5" stopIfTrue="1" operator="equal">
+      <formula>"USTERKA"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="0" priority="6" stopIfTrue="1" operator="equal">
+      <formula>"USTERKA PODRZĘDNA"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <dataValidations count="2">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="Q1:Q1048576" xr:uid="{EC584E36-1352-4872-B630-26EF7FB99641}">
+      <formula1>"BŁĄD KRYTYCZNY,BŁĄD ISTOTNY,BŁĄD,ISTOTNA USTERKA,USTERKA,USTERKA PODRZĘDNA"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B2:B1048576 O1:O1048576" xr:uid="{7ACD998E-99F8-4296-8618-35FF2D5CA65D}">
+      <formula1>"TAK,NIE"</formula1>
+    </dataValidation>
+  </dataValidations>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>